<commit_message>
modify the animation and proces and dump
</commit_message>
<xml_diff>
--- a/backend/pose/output/right-shoulder-angle-a.xlsx
+++ b/backend/pose/output/right-shoulder-angle-a.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.34375, 268.796875, 48.21875, 141.625, 0.9041695594787598, 329.0, 399.609375, 0.984375, 333.75, 394.21875, 0.96533203125, 322.75, 394.21875, 0.98046875, 339.25, 396.328125, 0.61474609375, 311.0, 395.15625, 0.75634765625, 351.0, 428.203125, 0.96875, 293.5, 426.5625, 0.97412109375, 357.5, 468.75, 0.888671875, 280.75, 465.0, 0.9189453125, 360.0, 504.375, 0.85595703125, 280.5, 501.5625, 0.884765625, 336.5, 505.3125, 0.96923828125, 301.5, 504.375, 0.9716796875, 332.0, 564.375, 0.93701171875, 299.75, 562.03125, 0.943359375, 325.0, 616.40625, 0.8857421875, 302.5, 616.875, 0.89306640625]]</t>
+          <t>[[0.0, 0.0, 160.34375, 268.796875, 48.21875, 141.625, 0.9041695594787598, 329.0, 399.375, 0.984375, 333.75, 394.21875, 0.96533203125, 322.75, 394.21875, 0.98046875, 339.25, 396.328125, 0.6142578125, 311.0, 395.15625, 0.7568359375, 351.0, 428.203125, 0.96875, 293.5, 426.5625, 0.97412109375, 357.5, 468.75, 0.888671875, 280.75, 465.0, 0.9189453125, 360.0, 504.375, 0.85595703125, 280.5, 501.5625, 0.884765625, 336.5, 505.3125, 0.96923828125, 301.5, 504.375, 0.9716796875, 332.0, 564.375, 0.93701171875, 299.75, 562.03125, 0.943359375, 325.0, 616.40625, 0.88525390625, 302.5, 616.875, 0.89306640625]]</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.5, 268.921875, 48.15625, 141.625, 0.9075307846069336, 328.0, 399.84375, 0.9833984375, 333.0, 394.6875, 0.96337890625, 322.0, 394.453125, 0.97900390625, 338.5, 396.5625, 0.61376953125, 310.5, 395.15625, 0.75146484375, 350.5, 428.4375, 0.96875, 293.0, 426.796875, 0.97412109375, 357.5, 468.75, 0.88916015625, 280.75, 465.46875, 0.91748046875, 360.5, 503.90625, 0.85595703125, 281.0, 502.03125, 0.8828125, 336.5, 505.78125, 0.96923828125, 301.5, 504.84375, 0.97216796875, 332.5, 564.84375, 0.93896484375, 300.0, 562.03125, 0.94482421875, 325.25, 616.875, 0.8916015625, 301.5, 615.9375, 0.8984375]]</t>
+          <t>[[0.0, 0.0, 160.5, 268.921875, 48.15625, 141.625, 0.9080109596252441, 328.0, 399.84375, 0.9833984375, 333.0, 394.6875, 0.96337890625, 322.0, 394.453125, 0.97900390625, 338.5, 396.5625, 0.6142578125, 310.5, 395.15625, 0.751953125, 350.5, 428.4375, 0.96875, 293.0, 426.796875, 0.97412109375, 357.5, 468.75, 0.88916015625, 280.75, 465.46875, 0.91748046875, 360.5, 503.90625, 0.85595703125, 281.0, 502.03125, 0.8828125, 336.5, 505.78125, 0.96923828125, 301.5, 504.84375, 0.97216796875, 332.25, 564.84375, 0.93896484375, 300.0, 562.03125, 0.94482421875, 325.25, 616.875, 0.8916015625, 301.5, 615.9375, 0.8984375]]</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.5625, 269.0, 48.28125, 141.625, 0.9075307846069336, 327.0, 400.3125, 0.98388671875, 332.0, 395.15625, 0.9638671875, 321.0, 394.6875, 0.9794921875, 337.5, 396.796875, 0.6103515625, 309.5, 395.625, 0.75, 349.75, 428.671875, 0.96875, 292.25, 427.265625, 0.97412109375, 357.5, 468.28125, 0.88916015625, 280.75, 465.46875, 0.91796875, 361.0, 502.5, 0.85595703125, 281.25, 501.09375, 0.88330078125, 336.5, 506.25, 0.9697265625, 301.5, 505.3125, 0.97216796875, 332.5, 564.84375, 0.93896484375, 300.0, 562.5, 0.94482421875, 325.5, 615.9375, 0.8916015625, 301.5, 614.53125, 0.89892578125]]</t>
+          <t>[[0.0, 0.0, 160.5625, 269.0, 48.28125, 141.625, 0.9075307846069336, 327.0, 400.3125, 0.98388671875, 332.0, 394.921875, 0.9638671875, 321.0, 394.6875, 0.9794921875, 337.5, 396.796875, 0.6103515625, 309.5, 395.625, 0.75, 349.75, 428.671875, 0.96875, 292.25, 427.265625, 0.97412109375, 357.5, 468.28125, 0.88916015625, 280.75, 465.46875, 0.91796875, 361.0, 502.5, 0.85595703125, 281.25, 501.09375, 0.88330078125, 336.5, 506.25, 0.9697265625, 301.5, 505.3125, 0.97216796875, 332.5, 564.84375, 0.939453125, 300.0, 562.5, 0.94482421875, 325.5, 615.9375, 0.8916015625, 301.5, 614.53125, 0.89892578125]]</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.46875, 269.078125, 48.28125, 141.625, 0.9065704345703125, 326.0, 400.546875, 0.9833984375, 331.0, 395.15625, 0.96630859375, 319.75, 395.15625, 0.97802734375, 336.75, 397.03125, 0.64990234375, 308.5, 396.09375, 0.73828125, 349.25, 428.4375, 0.96875, 291.75, 427.734375, 0.97412109375, 357.0, 467.34375, 0.89013671875, 280.0, 465.9375, 0.91748046875, 360.5, 502.03125, 0.85693359375, 281.5, 500.625, 0.88330078125, 336.5, 506.71875, 0.9697265625, 301.25, 505.78125, 0.97216796875, 333.0, 564.84375, 0.939453125, 300.0, 563.4375, 0.94482421875, 325.75, 616.40625, 0.89208984375, 301.25, 615.46875, 0.89892578125]]</t>
+          <t>[[0.0, 0.0, 160.46875, 269.078125, 48.28125, 141.625, 0.9065704345703125, 326.0, 400.3125, 0.9833984375, 331.0, 395.15625, 0.96630859375, 319.75, 395.15625, 0.97802734375, 336.75, 397.03125, 0.6494140625, 308.5, 396.09375, 0.73828125, 349.25, 428.4375, 0.96875, 291.5, 427.734375, 0.97412109375, 357.25, 467.34375, 0.89013671875, 280.0, 465.9375, 0.91748046875, 360.5, 502.03125, 0.85693359375, 281.5, 501.09375, 0.88330078125, 336.5, 506.71875, 0.9697265625, 301.25, 505.78125, 0.97216796875, 333.0, 564.84375, 0.939453125, 300.0, 563.4375, 0.94482421875, 325.75, 616.40625, 0.89208984375, 301.5, 615.46875, 0.89892578125]]</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.59375, 269.3125, 48.15625, 141.25, 0.9051299095153809, 325.0, 400.78125, 0.9833984375, 329.75, 395.625, 0.9658203125, 318.75, 395.625, 0.97802734375, 335.75, 397.5, 0.64697265625, 307.5, 396.796875, 0.73486328125, 348.75, 428.203125, 0.96875, 290.75, 428.4375, 0.9736328125, 357.0, 466.40625, 0.890625, 279.75, 466.875, 0.91552734375, 360.0, 501.09375, 0.857421875, 282.25, 501.09375, 0.88037109375, 337.0, 506.71875, 0.96923828125, 301.5, 506.25, 0.9716796875, 334.0, 565.3125, 0.9384765625, 300.0, 563.90625, 0.943359375, 325.5, 616.875, 0.89111328125, 301.25, 615.9375, 0.89697265625]]</t>
+          <t>[[0.0, 0.0, 160.59375, 269.296875, 48.15625, 141.25, 0.9051299095153809, 325.0, 400.78125, 0.98291015625, 329.75, 395.625, 0.9658203125, 318.75, 395.625, 0.97802734375, 335.75, 397.5, 0.646484375, 307.5, 397.03125, 0.73486328125, 348.75, 428.203125, 0.96875, 290.75, 428.4375, 0.9736328125, 357.0, 466.40625, 0.890625, 279.75, 466.875, 0.91552734375, 360.0, 501.09375, 0.857421875, 282.25, 501.09375, 0.88037109375, 337.0, 506.71875, 0.96923828125, 301.5, 506.25, 0.9716796875, 334.0, 565.3125, 0.9384765625, 300.0, 563.90625, 0.943359375, 325.5, 616.875, 0.890625, 301.25, 615.9375, 0.89697265625]]</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.40625, 269.390625, 48.15625, 140.25, 0.9051299095153809, 324.0, 401.71875, 0.98291015625, 329.0, 396.5625, 0.9658203125, 317.5, 396.5625, 0.978515625, 335.0, 398.4375, 0.6416015625, 306.25, 397.96875, 0.734375, 348.0, 428.671875, 0.96875, 289.75, 429.609375, 0.97314453125, 356.0, 466.40625, 0.89208984375, 279.5, 468.515625, 0.9130859375, 360.0, 501.09375, 0.8583984375, 282.0, 504.375, 0.876953125, 336.5, 506.71875, 0.96923828125, 301.0, 506.71875, 0.9716796875, 334.0, 565.3125, 0.9384765625, 299.5, 564.375, 0.94287109375, 325.75, 617.8125, 0.890625, 300.75, 616.40625, 0.89599609375]]</t>
+          <t>[[0.0, 0.0, 160.40625, 269.390625, 48.21875, 140.25, 0.9051299095153809, 324.0, 401.71875, 0.98291015625, 329.0, 396.5625, 0.9658203125, 317.5, 396.5625, 0.978515625, 335.0, 398.4375, 0.64111328125, 306.25, 397.96875, 0.73486328125, 348.0, 428.671875, 0.96875, 289.5, 429.609375, 0.97314453125, 356.0, 466.40625, 0.89208984375, 279.5, 468.515625, 0.9130859375, 360.0, 501.09375, 0.8583984375, 282.0, 504.375, 0.876953125, 336.5, 506.71875, 0.96923828125, 301.0, 506.71875, 0.9716796875, 334.0, 565.3125, 0.9384765625, 299.5, 564.375, 0.94287109375, 325.75, 617.8125, 0.890625, 300.5, 616.40625, 0.896484375]]</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.25, 269.71875, 48.15625, 139.0, 0.9065704345703125, 323.0, 403.125, 0.9833984375, 328.0, 397.734375, 0.96728515625, 317.0, 397.96875, 0.97900390625, 334.0, 399.609375, 0.6572265625, 305.5, 399.140625, 0.73974609375, 347.0, 429.140625, 0.96875, 288.75, 430.546875, 0.9736328125, 355.25, 466.640625, 0.8916015625, 279.0, 469.6875, 0.91650390625, 359.75, 501.5625, 0.85888671875, 284.0, 505.78125, 0.8818359375, 337.5, 507.1875, 0.96923828125, 301.5, 508.125, 0.97119140625, 338.0, 564.375, 0.9365234375, 300.0, 564.375, 0.94189453125, 326.5, 616.875, 0.88623046875, 301.0, 615.9375, 0.89306640625]]</t>
+          <t>[[0.0, 0.0, 160.25, 269.703125, 48.15625, 139.0, 0.9065704345703125, 323.0, 403.125, 0.9833984375, 328.0, 397.734375, 0.96728515625, 317.0, 397.96875, 0.97900390625, 334.0, 399.609375, 0.658203125, 305.5, 399.140625, 0.73974609375, 347.0, 429.140625, 0.96875, 288.75, 430.546875, 0.9736328125, 355.25, 466.640625, 0.8916015625, 279.0, 469.6875, 0.91650390625, 359.75, 501.5625, 0.85888671875, 284.0, 505.78125, 0.8818359375, 337.5, 507.1875, 0.96923828125, 301.5, 508.125, 0.97119140625, 338.0, 564.375, 0.93701171875, 300.0, 564.375, 0.94189453125, 326.5, 616.875, 0.88671875, 301.0, 615.9375, 0.89306640625]]</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 159.90625, 270.28125, 48.28125, 138.125, 0.906090259552002, 322.5, 406.40625, 0.982421875, 327.25, 401.015625, 0.96044921875, 316.0, 400.78125, 0.98046875, 332.75, 402.65625, 0.5712890625, 304.0, 401.71875, 0.75390625, 345.0, 430.78125, 0.96826171875, 287.5, 432.890625, 0.97265625, 354.5, 466.40625, 0.88916015625, 278.5, 469.6875, 0.90966796875, 359.75, 500.625, 0.853515625, 286.25, 500.625, 0.8720703125, 337.0, 508.125, 0.96875, 300.75, 509.0625, 0.97021484375, 342.75, 563.4375, 0.9365234375, 299.5, 564.84375, 0.94091796875, 326.25, 615.46875, 0.888671875, 300.25, 615.46875, 0.89404296875]]</t>
+          <t>[[0.0, 0.0, 159.90625, 270.28125, 48.28125, 138.125, 0.9056100845336914, 322.5, 406.40625, 0.982421875, 327.25, 401.015625, 0.96044921875, 316.0, 400.78125, 0.98046875, 332.75, 402.65625, 0.57177734375, 304.0, 401.71875, 0.75390625, 345.0, 430.78125, 0.96826171875, 287.5, 432.890625, 0.97265625, 354.5, 466.40625, 0.88916015625, 278.5, 469.6875, 0.90966796875, 359.75, 500.625, 0.853515625, 286.25, 500.625, 0.8720703125, 337.0, 508.125, 0.96875, 300.75, 509.0625, 0.97021484375, 342.75, 563.4375, 0.9365234375, 299.25, 564.84375, 0.94091796875, 326.0, 615.46875, 0.888671875, 300.25, 615.46875, 0.89404296875]]</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 159.53125, 271.53125, 48.28125, 136.5, 0.9046497344970703, 322.0, 409.453125, 0.9814453125, 326.5, 404.0625, 0.95458984375, 315.5, 404.0625, 0.98046875, 331.75, 405.9375, 0.521484375, 303.25, 405.234375, 0.7705078125, 344.0, 432.1875, 0.96875, 287.0, 435.46875, 0.9736328125, 354.0, 466.640625, 0.8896484375, 278.0, 472.265625, 0.9189453125, 359.0, 500.625, 0.85595703125, 288.5, 503.90625, 0.884765625, 337.5, 509.53125, 0.96875, 301.0, 510.9375, 0.97119140625, 345.75, 562.5, 0.93603515625, 299.0, 565.3125, 0.94189453125, 326.0, 615.0, 0.88720703125, 299.75, 615.9375, 0.89453125]]</t>
+          <t>[[0.0, 0.0, 159.53125, 271.53125, 48.28125, 136.5, 0.9046497344970703, 322.0, 409.21875, 0.9814453125, 326.5, 404.0625, 0.95458984375, 315.5, 404.0625, 0.98046875, 331.75, 405.9375, 0.52197265625, 303.25, 405.234375, 0.7705078125, 344.0, 432.1875, 0.96875, 287.0, 435.46875, 0.9736328125, 354.0, 466.640625, 0.8896484375, 278.0, 472.265625, 0.9189453125, 359.0, 500.625, 0.85595703125, 288.5, 503.90625, 0.884765625, 337.5, 509.53125, 0.96875, 301.0, 510.9375, 0.97119140625, 345.75, 562.5, 0.93603515625, 299.0, 565.3125, 0.94189453125, 326.0, 615.0, 0.8876953125, 299.75, 615.9375, 0.89501953125]]</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 159.28125, 272.59375, 48.28125, 135.875, 0.907050609588623, 321.0, 412.265625, 0.982421875, 325.75, 407.109375, 0.94873046875, 314.75, 407.109375, 0.98291015625, 331.5, 408.515625, 0.428955078125, 302.75, 408.046875, 0.77197265625, 343.25, 433.828125, 0.97265625, 287.0, 438.75, 0.970703125, 354.5, 467.8125, 0.9052734375, 277.5, 477.65625, 0.90673828125, 359.0, 500.625, 0.87060546875, 291.75, 509.0625, 0.8759765625, 337.0, 510.46875, 0.970703125, 301.25, 512.34375, 0.96923828125, 346.25, 563.4375, 0.9404296875, 298.5, 565.78125, 0.939453125, 326.75, 616.40625, 0.89404296875, 299.0, 614.0625, 0.8916015625]]</t>
+          <t>[[0.0, 0.0, 159.2734375, 272.59375, 48.28125, 135.875, 0.907050609588623, 321.0, 412.265625, 0.982421875, 325.75, 406.875, 0.94873046875, 314.75, 407.109375, 0.98291015625, 331.5, 408.515625, 0.4287109375, 302.75, 408.046875, 0.77197265625, 343.25, 433.828125, 0.97265625, 287.0, 438.75, 0.970703125, 354.5, 467.8125, 0.9052734375, 277.5, 477.65625, 0.90673828125, 359.0, 500.625, 0.87060546875, 291.75, 509.0625, 0.8759765625, 337.0, 510.46875, 0.970703125, 301.25, 512.34375, 0.96923828125, 346.25, 563.4375, 0.9404296875, 298.5, 565.78125, 0.939453125, 326.75, 616.40625, 0.89404296875, 299.0, 614.0625, 0.8916015625]]</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 158.9453125, 273.0, 47.90625, 134.75, 0.9065704345703125, 321.0, 414.84375, 0.9794921875, 325.75, 409.6875, 0.94189453125, 314.75, 409.6875, 0.98046875, 331.5, 410.625, 0.419921875, 302.5, 410.15625, 0.767578125, 343.25, 435.234375, 0.97216796875, 287.0, 440.625, 0.97021484375, 355.0, 468.28125, 0.904296875, 277.25, 478.828125, 0.90380859375, 358.5, 500.625, 0.86865234375, 291.0, 509.0625, 0.87158203125, 336.75, 511.875, 0.97021484375, 301.0, 513.75, 0.96875, 345.75, 563.90625, 0.939453125, 298.5, 567.65625, 0.9384765625, 327.25, 617.34375, 0.89306640625, 298.75, 614.0625, 0.89013671875]]</t>
+          <t>[[0.0, 0.0, 158.9453125, 273.0, 47.90625, 134.75, 0.9065704345703125, 321.0, 414.84375, 0.9794921875, 325.75, 409.6875, 0.94189453125, 314.75, 409.6875, 0.98046875, 331.5, 410.625, 0.419921875, 302.5, 410.15625, 0.767578125, 343.25, 435.234375, 0.97216796875, 287.0, 440.625, 0.97021484375, 355.0, 468.28125, 0.904296875, 277.25, 478.828125, 0.90380859375, 358.5, 500.625, 0.86865234375, 291.0, 509.0625, 0.87158203125, 336.75, 511.875, 0.97021484375, 301.0, 513.75, 0.96875, 345.75, 563.90625, 0.939453125, 298.5, 567.65625, 0.93798828125, 327.5, 617.34375, 0.89306640625, 298.75, 614.0625, 0.89013671875]]</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 158.890625, 273.3125, 47.5625, 134.375, 0.9094514846801758, 322.0, 416.71875, 0.98095703125, 326.5, 411.09375, 0.9462890625, 315.5, 411.5625, 0.982421875, 332.5, 412.03125, 0.421142578125, 303.25, 411.796875, 0.77099609375, 344.5, 435.703125, 0.97216796875, 287.75, 441.5625, 0.970703125, 355.0, 467.8125, 0.904296875, 277.5, 479.765625, 0.90576171875, 357.5, 500.15625, 0.869140625, 293.5, 509.53125, 0.87451171875, 336.5, 511.40625, 0.9697265625, 301.0, 513.28125, 0.96826171875, 346.25, 563.4375, 0.9384765625, 299.0, 566.71875, 0.9375, 327.5, 616.40625, 0.890625, 298.0, 612.1875, 0.8876953125]]</t>
+          <t>[[0.0, 0.0, 158.890625, 273.3125, 47.5625, 134.375, 0.9094514846801758, 322.0, 416.71875, 0.98095703125, 326.5, 411.09375, 0.9462890625, 315.5, 411.5625, 0.982421875, 332.5, 412.03125, 0.4208984375, 303.25, 411.796875, 0.77099609375, 344.5, 435.703125, 0.97216796875, 287.75, 441.5625, 0.970703125, 355.0, 467.8125, 0.904296875, 277.5, 480.0, 0.90576171875, 357.5, 500.15625, 0.869140625, 293.5, 509.53125, 0.87451171875, 336.5, 511.40625, 0.9697265625, 301.0, 513.28125, 0.96826171875, 346.25, 563.4375, 0.9384765625, 299.0, 566.71875, 0.9375, 327.5, 616.40625, 0.890625, 298.0, 612.1875, 0.8876953125]]</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 158.921875, 273.4375, 46.71875, 134.5, 0.9089713096618652, 322.25, 416.71875, 0.98046875, 327.0, 411.5625, 0.9462890625, 316.0, 411.5625, 0.9814453125, 333.0, 412.03125, 0.424560546875, 304.0, 411.5625, 0.7646484375, 345.0, 435.0, 0.970703125, 288.75, 441.09375, 0.97021484375, 355.5, 466.171875, 0.89697265625, 278.5, 479.53125, 0.90625, 357.5, 497.34375, 0.85888671875, 296.25, 507.1875, 0.87451171875, 337.0, 510.9375, 0.96923828125, 301.75, 513.28125, 0.96875, 346.25, 563.4375, 0.93896484375, 298.75, 567.65625, 0.939453125, 328.0, 615.9375, 0.89404296875, 298.5, 616.875, 0.89306640625]]</t>
+          <t>[[0.0, 0.0, 158.8984375, 273.4375, 46.71875, 134.5, 0.9089713096618652, 322.25, 416.71875, 0.98046875, 326.75, 411.5625, 0.9462890625, 316.0, 411.5625, 0.9814453125, 333.0, 412.03125, 0.42431640625, 304.0, 411.5625, 0.76513671875, 345.0, 435.0, 0.970703125, 288.75, 441.328125, 0.97021484375, 355.5, 466.171875, 0.89697265625, 278.5, 479.53125, 0.90625, 357.5, 497.34375, 0.85888671875, 296.25, 507.1875, 0.87451171875, 337.0, 510.9375, 0.96923828125, 301.75, 513.28125, 0.96875, 346.25, 563.4375, 0.93896484375, 298.75, 567.65625, 0.939453125, 328.0, 615.9375, 0.89453125, 298.5, 616.875, 0.89306640625]]</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 158.7421875, 273.125, 46.5, 134.75, 0.9080109596252441, 323.5, 416.015625, 0.9814453125, 328.25, 410.390625, 0.94873046875, 317.25, 410.859375, 0.98193359375, 334.75, 410.625, 0.429931640625, 305.25, 410.859375, 0.7626953125, 346.25, 433.359375, 0.97021484375, 290.0, 440.390625, 0.97021484375, 355.5, 462.65625, 0.89306640625, 278.5, 478.828125, 0.908203125, 357.5, 492.65625, 0.8544921875, 298.25, 506.25, 0.87646484375, 338.0, 510.0, 0.96923828125, 302.5, 511.875, 0.96923828125, 346.0, 562.5, 0.93994140625, 298.5, 566.71875, 0.94140625, 328.0, 614.53125, 0.8974609375, 298.5, 616.875, 0.89794921875]]</t>
+          <t>[[0.0, 0.0, 158.7421875, 273.125, 46.5, 134.75, 0.9080109596252441, 323.5, 416.015625, 0.9814453125, 328.25, 410.390625, 0.94873046875, 317.25, 410.859375, 0.98193359375, 334.5, 410.625, 0.429931640625, 305.25, 410.859375, 0.7626953125, 346.25, 433.359375, 0.97021484375, 290.0, 440.390625, 0.97021484375, 355.5, 462.65625, 0.892578125, 278.5, 478.828125, 0.908203125, 357.5, 492.65625, 0.8544921875, 298.25, 506.25, 0.87646484375, 338.0, 510.0, 0.96923828125, 302.5, 511.875, 0.96923828125, 346.0, 562.5, 0.93994140625, 298.5, 566.71875, 0.94140625, 328.25, 614.53125, 0.8974609375, 298.5, 616.875, 0.89794921875]]</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 158.8984375, 272.71875, 46.71875, 135.25, 0.9046497344970703, 326.5, 414.84375, 0.982421875, 331.25, 409.21875, 0.94921875, 320.0, 409.6875, 0.98388671875, 337.5, 409.21875, 0.405029296875, 307.75, 409.21875, 0.771484375, 348.0, 431.953125, 0.96826171875, 291.25, 438.75, 0.97021484375, 356.0, 459.84375, 0.876953125, 278.75, 476.953125, 0.9091796875, 357.0, 489.84375, 0.83349609375, 298.5, 505.78125, 0.87646484375, 339.0, 508.59375, 0.96826171875, 303.25, 510.9375, 0.96875, 346.75, 561.09375, 0.93896484375, 299.5, 565.78125, 0.94287109375, 329.75, 612.65625, 0.900390625, 298.75, 616.40625, 0.9033203125]]</t>
+          <t>[[0.0, 0.0, 158.890625, 272.71875, 46.71875, 135.25, 0.9051299095153809, 326.5, 414.84375, 0.982421875, 331.25, 409.21875, 0.94921875, 320.0, 409.6875, 0.98388671875, 337.5, 409.21875, 0.40478515625, 307.75, 409.21875, 0.771484375, 348.0, 431.953125, 0.96826171875, 291.25, 438.75, 0.97021484375, 356.0, 459.84375, 0.876953125, 278.75, 476.953125, 0.9091796875, 357.0, 489.84375, 0.83349609375, 298.5, 505.3125, 0.87646484375, 339.0, 508.59375, 0.96826171875, 303.25, 510.9375, 0.96875, 347.0, 561.09375, 0.93896484375, 299.5, 565.78125, 0.943359375, 329.75, 612.65625, 0.900390625, 298.75, 616.40625, 0.9033203125]]</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 158.9375, 272.5, 47.1875, 135.5, 0.9051299095153809, 329.5, 414.140625, 0.984375, 334.25, 408.515625, 0.95361328125, 323.0, 408.75, 0.986328125, 340.5, 408.28125, 0.398681640625, 310.25, 408.28125, 0.7802734375, 350.0, 430.78125, 0.9677734375, 293.75, 437.34375, 0.970703125, 355.0, 459.609375, 0.87646484375, 278.5, 475.3125, 0.9111328125, 356.5, 490.3125, 0.83349609375, 298.5, 505.3125, 0.87890625, 340.75, 508.125, 0.96826171875, 305.0, 510.0, 0.96923828125, 348.25, 560.625, 0.93798828125, 301.0, 564.84375, 0.9423828125, 332.0, 615.0, 0.896484375, 298.5, 616.875, 0.89990234375]]</t>
+          <t>[[0.0, 0.0, 158.9375, 272.5, 47.1875, 135.5, 0.9051299095153809, 329.5, 414.140625, 0.984375, 334.25, 408.515625, 0.95361328125, 323.0, 408.75, 0.986328125, 340.5, 408.28125, 0.3994140625, 310.5, 408.28125, 0.7802734375, 350.0, 430.78125, 0.9677734375, 293.75, 437.34375, 0.970703125, 355.0, 459.609375, 0.87646484375, 278.5, 475.3125, 0.9111328125, 356.5, 490.3125, 0.83349609375, 298.5, 505.3125, 0.87890625, 340.75, 508.125, 0.96826171875, 305.0, 510.0, 0.96923828125, 348.25, 560.625, 0.93798828125, 301.0, 564.84375, 0.9423828125, 332.0, 615.0, 0.896484375, 298.5, 616.875, 0.900390625]]</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 159.46875, 272.6875, 47.5625, 135.625, 0.9027290344238281, 332.0, 414.375, 0.9833984375, 336.5, 408.75, 0.94970703125, 325.5, 409.21875, 0.98583984375, 342.25, 408.75, 0.377685546875, 312.5, 408.75, 0.78076171875, 351.5, 430.3125, 0.96923828125, 295.75, 436.875, 0.97119140625, 356.5, 457.96875, 0.88671875, 278.75, 474.140625, 0.912109375, 357.0, 487.5, 0.84765625, 298.75, 503.90625, 0.8818359375, 342.25, 507.1875, 0.9697265625, 306.75, 509.53125, 0.97021484375, 350.0, 561.5625, 0.94140625, 302.5, 565.3125, 0.94482421875, 335.0, 617.8125, 0.900390625, 299.0, 618.75, 0.90283203125]]</t>
+          <t>[[0.0, 0.0, 159.4765625, 272.6875, 47.5625, 135.625, 0.9027290344238281, 332.0, 414.375, 0.9833984375, 336.5, 408.75, 0.94970703125, 325.5, 408.984375, 0.98583984375, 342.25, 408.75, 0.377685546875, 312.5, 408.75, 0.78076171875, 351.5, 430.3125, 0.96923828125, 295.75, 436.875, 0.97119140625, 356.5, 457.96875, 0.88671875, 278.75, 474.140625, 0.91259765625, 357.0, 487.5, 0.84765625, 298.75, 503.90625, 0.8818359375, 342.25, 507.1875, 0.9697265625, 306.75, 509.53125, 0.97021484375, 350.0, 561.5625, 0.94140625, 302.5, 565.3125, 0.94482421875, 335.0, 617.8125, 0.900390625, 299.0, 618.75, 0.90283203125]]</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 160.0625, 273.0625, 47.90625, 135.25, 0.9008083343505859, 335.0, 415.3125, 0.9814453125, 339.25, 409.6875, 0.9384765625, 328.5, 410.15625, 0.9853515625, 344.25, 409.6875, 0.32275390625, 315.5, 410.15625, 0.78857421875, 353.5, 430.78125, 0.96337890625, 298.0, 437.578125, 0.9697265625, 359.25, 457.265625, 0.84716796875, 278.75, 472.96875, 0.91015625, 357.25, 486.09375, 0.7958984375, 299.0, 502.03125, 0.875, 343.5, 507.1875, 0.9658203125, 307.75, 509.0625, 0.96875, 351.75, 561.5625, 0.9365234375, 303.25, 565.78125, 0.94482421875, 338.0, 617.34375, 0.900390625, 300.0, 619.6875, 0.908203125]]</t>
+          <t>[[0.0, 0.0, 159.8125, 273.03125, 47.75, 134.75, 0.9008083343505859, 335.0, 415.3125, 0.98291015625, 339.5, 409.6875, 0.94775390625, 328.5, 410.15625, 0.98388671875, 344.25, 409.6875, 0.435302734375, 315.25, 410.15625, 0.7880859375, 353.5, 430.546875, 0.95849609375, 297.75, 437.578125, 0.97216796875, 358.75, 456.796875, 0.8271484375, 278.5, 472.734375, 0.919921875, 356.25, 486.09375, 0.78076171875, 297.75, 502.03125, 0.88134765625, 343.25, 507.1875, 0.96240234375, 307.5, 509.53125, 0.96923828125, 351.25, 561.5625, 0.927734375, 303.25, 565.78125, 0.943359375, 337.5, 617.34375, 0.88525390625, 300.0, 619.6875, 0.90234375]]</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 161.3125, 273.875, 50.90625, 133.875, 0.8945660591125488, 338.25, 418.125, 0.984375, 343.0, 412.5, 0.953125, 331.5, 412.734375, 0.9853515625, 348.25, 413.4375, 0.46044921875, 318.25, 412.96875, 0.794921875, 356.25, 433.59375, 0.931640625, 301.0, 439.6875, 0.97021484375, 368.5, 448.125, 0.63525390625, 278.5, 473.671875, 0.9169921875, 365.5, 459.375, 0.5673828125, 298.75, 502.03125, 0.86328125, 345.25, 509.0625, 0.94482421875, 309.25, 510.46875, 0.96435546875, 353.0, 562.96875, 0.904296875, 304.5, 565.78125, 0.94287109375, 340.5, 620.625, 0.87353515625, 300.25, 619.6875, 0.91162109375]]</t>
+          <t>[[0.0, 0.0, 161.3125, 273.875, 50.90625, 133.875, 0.8945660591125488, 338.25, 418.125, 0.984375, 343.0, 412.5, 0.953125, 331.5, 412.734375, 0.9853515625, 348.25, 413.4375, 0.4609375, 318.25, 412.96875, 0.79541015625, 356.25, 433.59375, 0.931640625, 301.0, 439.921875, 0.97021484375, 368.5, 448.125, 0.63525390625, 278.5, 473.671875, 0.9169921875, 365.5, 459.609375, 0.56787109375, 298.75, 502.03125, 0.86328125, 345.25, 509.0625, 0.94482421875, 309.25, 510.46875, 0.96435546875, 353.0, 562.96875, 0.904296875, 304.5, 565.78125, 0.94287109375, 340.5, 620.625, 0.8740234375, 300.25, 619.6875, 0.91162109375]]</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 161.90625, 274.46875, 49.9375, 133.125, 0.8998479843139648, 340.0, 420.46875, 0.982421875, 345.0, 415.3125, 0.9541015625, 333.75, 415.3125, 0.98046875, 350.5, 416.25, 0.54345703125, 322.25, 416.25, 0.759765625, 359.25, 437.109375, 0.958984375, 305.0, 441.796875, 0.97216796875, 366.25, 461.953125, 0.8369140625, 280.5, 475.078125, 0.919921875, 363.0, 491.25, 0.79296875, 299.5, 503.90625, 0.880859375, 346.25, 510.9375, 0.96240234375, 311.0, 512.34375, 0.96923828125, 355.25, 565.3125, 0.9287109375, 305.25, 566.71875, 0.94287109375, 342.0, 621.5625, 0.88623046875, 301.0, 617.8125, 0.90234375]]</t>
+          <t>[[0.0, 0.0, 161.90625, 274.46875, 49.9375, 133.125, 0.8998479843139648, 340.0, 420.46875, 0.982421875, 345.0, 415.3125, 0.9541015625, 333.75, 415.3125, 0.98046875, 350.5, 416.25, 0.54345703125, 322.25, 416.25, 0.759765625, 359.25, 437.109375, 0.958984375, 305.0, 441.796875, 0.97216796875, 366.25, 461.953125, 0.8369140625, 280.5, 475.078125, 0.919921875, 363.0, 491.25, 0.79296875, 299.5, 503.90625, 0.88134765625, 346.25, 510.9375, 0.96240234375, 311.0, 512.34375, 0.96923828125, 355.25, 565.3125, 0.9287109375, 305.25, 566.71875, 0.94287109375, 342.0, 621.5625, 0.88623046875, 301.0, 617.8125, 0.90234375]]</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 164.609375, 275.5703125, 49.75, 131.25, 0.9061203002929688, 344.25, 423.75, 0.97802734375, 348.75, 417.65625, 0.9541015625, 337.75, 418.59375, 0.9775390625, 354.5, 419.0625, 0.468017578125, 325.75, 420.703125, 0.80908203125, 362.0, 442.03125, 0.97119140625, 310.5, 444.84375, 0.974609375, 370.25, 464.53125, 0.88525390625, 285.25, 475.3125, 0.9326171875, 367.5, 493.125, 0.85595703125, 299.0, 505.78125, 0.90869140625, 348.0, 514.21875, 0.97265625, 314.75, 514.6875, 0.97412109375, 356.0, 567.65625, 0.94189453125, 307.5, 567.65625, 0.9482421875, 343.25, 622.03125, 0.89013671875, 301.25, 617.8125, 0.89892578125]]</t>
+          <t>[[0.0, 0.0, 164.609375, 275.5703125, 49.75, 131.25, 0.9061203002929688, 344.25, 423.75, 0.97802734375, 348.75, 417.65625, 0.9541015625, 337.75, 418.59375, 0.9775390625, 354.5, 419.0625, 0.468017578125, 325.75, 420.703125, 0.80908203125, 362.0, 442.03125, 0.97119140625, 310.5, 444.84375, 0.974609375, 370.25, 464.53125, 0.88525390625, 285.0, 475.3125, 0.9326171875, 367.5, 493.125, 0.85595703125, 299.0, 505.78125, 0.90869140625, 348.0, 514.21875, 0.97265625, 314.75, 514.6875, 0.97412109375, 356.0, 567.65625, 0.94189453125, 307.5, 567.65625, 0.9482421875, 343.25, 622.03125, 0.89013671875, 301.25, 617.8125, 0.89892578125]]</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 165.5703125, 276.4140625, 49.875, 129.75, 0.9181187152862549, 346.0, 426.328125, 0.98046875, 351.0, 420.46875, 0.96435546875, 339.5, 420.9375, 0.978515625, 357.0, 422.34375, 0.544921875, 328.25, 422.8125, 0.798828125, 364.75, 447.1875, 0.9736328125, 312.5, 448.125, 0.97607421875, 371.5, 472.5, 0.89990234375, 288.25, 477.421875, 0.9375, 370.25, 502.5, 0.8740234375, 299.75, 508.125, 0.916015625, 350.25, 518.90625, 0.97412109375, 316.75, 518.4375, 0.9755859375, 356.0, 571.40625, 0.943359375, 308.25, 570.9375, 0.9482421875, 343.0, 622.5, 0.8896484375, 302.0, 617.34375, 0.896484375]]</t>
+          <t>[[0.0, 0.0, 165.5703125, 276.421875, 49.9375, 129.75, 0.9181187152862549, 346.0, 426.328125, 0.98046875, 351.0, 420.46875, 0.96484375, 339.5, 420.9375, 0.978515625, 357.0, 422.34375, 0.544921875, 328.25, 422.8125, 0.798828125, 364.75, 447.1875, 0.9736328125, 312.5, 448.125, 0.97607421875, 371.5, 472.5, 0.89990234375, 288.25, 477.421875, 0.9375, 370.25, 502.5, 0.87353515625, 299.75, 508.125, 0.916015625, 350.25, 518.90625, 0.97412109375, 316.75, 518.4375, 0.9755859375, 356.0, 571.40625, 0.943359375, 308.25, 570.9375, 0.9482421875, 343.0, 622.5, 0.8896484375, 302.0, 617.34375, 0.896484375]]</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 169.328125, 277.0, 54.9375, 128.375, 0.9056403636932373, 350.0, 428.203125, 0.978515625, 355.25, 422.578125, 0.9638671875, 343.5, 422.8125, 0.978515625, 361.75, 424.921875, 0.552734375, 331.75, 424.6875, 0.802734375, 368.0, 451.171875, 0.97265625, 315.5, 450.9375, 0.9765625, 378.75, 478.828125, 0.8798828125, 292.5, 481.40625, 0.93359375, 376.75, 510.46875, 0.84619140625, 301.0, 514.6875, 0.9072265625, 353.5, 521.25, 0.97216796875, 319.25, 520.78125, 0.97412109375, 356.25, 573.75, 0.94140625, 310.75, 573.75, 0.9482421875, 342.5, 622.96875, 0.8935546875, 302.75, 618.28125, 0.90283203125]]</t>
+          <t>[[0.0, 0.0, 169.328125, 277.0078125, 54.9375, 128.375, 0.9056403636932373, 350.0, 428.203125, 0.978515625, 355.25, 422.578125, 0.9638671875, 343.5, 423.046875, 0.978515625, 361.75, 424.921875, 0.552734375, 331.75, 424.6875, 0.802734375, 368.0, 451.171875, 0.97265625, 315.5, 450.9375, 0.9765625, 378.75, 478.828125, 0.88037109375, 292.25, 481.40625, 0.93359375, 376.75, 510.46875, 0.84619140625, 301.0, 514.6875, 0.9072265625, 353.5, 521.25, 0.97216796875, 319.25, 520.78125, 0.97412109375, 356.25, 573.75, 0.94140625, 310.75, 573.75, 0.94873046875, 342.5, 622.96875, 0.89404296875, 302.75, 618.28125, 0.90283203125]]</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 169.609375, 277.6171875, 52.8125, 127.3125, 0.9109196662902832, 353.75, 430.78125, 0.97607421875, 358.75, 425.390625, 0.95263671875, 347.25, 425.625, 0.97705078125, 364.5, 427.5, 0.449462890625, 335.5, 426.328125, 0.81298828125, 371.75, 453.28125, 0.97705078125, 317.25, 453.046875, 0.97900390625, 380.5, 483.28125, 0.9189453125, 295.75, 485.625, 0.94775390625, 379.5, 517.03125, 0.896484375, 300.75, 521.25, 0.9296875, 355.0, 521.71875, 0.9765625, 320.75, 521.25, 0.97705078125, 358.5, 575.15625, 0.943359375, 314.0, 576.09375, 0.947265625, 342.25, 622.96875, 0.8798828125, 305.25, 615.9375, 0.88623046875]]</t>
+          <t>[[0.0, 0.0, 169.609375, 277.6171875, 52.8125, 127.3125, 0.9109196662902832, 353.75, 430.78125, 0.97607421875, 358.75, 425.390625, 0.95263671875, 347.25, 425.625, 0.97705078125, 364.5, 427.5, 0.449462890625, 335.5, 426.328125, 0.81298828125, 371.75, 453.28125, 0.97705078125, 317.25, 452.8125, 0.97900390625, 380.5, 483.28125, 0.9189453125, 295.75, 485.625, 0.94775390625, 379.5, 517.03125, 0.896484375, 300.75, 521.25, 0.9296875, 355.0, 521.71875, 0.9765625, 320.75, 521.25, 0.97705078125, 358.5, 575.15625, 0.943359375, 314.0, 576.09375, 0.947265625, 342.25, 622.96875, 0.8798828125, 305.25, 615.9375, 0.88623046875]]</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 170.4375, 278.5078125, 54.65625, 126.1875, 0.9142792224884033, 356.0, 431.484375, 0.98095703125, 361.0, 426.328125, 0.9609375, 349.75, 426.328125, 0.98046875, 366.75, 428.90625, 0.4912109375, 338.75, 427.734375, 0.80615234375, 376.0, 455.15625, 0.97900390625, 320.25, 453.515625, 0.98046875, 385.5, 487.96875, 0.9267578125, 295.75, 484.21875, 0.953125, 384.5, 520.78125, 0.9072265625, 299.0, 517.96875, 0.93798828125, 357.25, 523.125, 0.978515625, 322.75, 522.1875, 0.97900390625, 360.0, 577.03125, 0.94677734375, 321.25, 575.625, 0.95068359375, 342.0, 624.84375, 0.88818359375, 309.75, 601.875, 0.89453125]]</t>
+          <t>[[0.0, 0.0, 170.4375, 278.5078125, 54.65625, 126.1875, 0.9142792224884033, 356.0, 431.484375, 0.98095703125, 361.0, 426.328125, 0.9609375, 349.75, 426.328125, 0.98046875, 366.75, 428.90625, 0.4921875, 338.75, 427.734375, 0.80615234375, 376.0, 455.15625, 0.97900390625, 320.25, 453.515625, 0.98046875, 385.5, 487.96875, 0.9267578125, 295.75, 484.21875, 0.953125, 384.5, 520.78125, 0.9072265625, 299.0, 517.96875, 0.93798828125, 357.25, 523.125, 0.978515625, 322.75, 522.1875, 0.97900390625, 360.0, 577.03125, 0.94677734375, 321.25, 575.625, 0.95068359375, 342.0, 624.84375, 0.88818359375, 309.75, 601.875, 0.89453125]]</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 171.59375, 278.6953125, 56.90625, 127.3125, 0.9133193492889404, 358.25, 431.484375, 0.982421875, 363.25, 426.328125, 0.96435546875, 352.0, 426.09375, 0.98095703125, 368.75, 428.671875, 0.52197265625, 341.25, 427.03125, 0.80078125, 378.75, 455.625, 0.97900390625, 323.5, 451.875, 0.98095703125, 391.0, 489.84375, 0.92578125, 296.25, 480.9375, 0.95361328125, 389.75, 520.3125, 0.90576171875, 300.0, 515.15625, 0.9375, 359.5, 524.53125, 0.9794921875, 325.25, 522.65625, 0.97998046875, 361.5, 581.25, 0.95068359375, 331.25, 577.96875, 0.95458984375, 340.5, 625.3125, 0.89892578125, 316.0, 600.0, 0.90576171875]]</t>
+          <t>[[0.0, 0.0, 171.59375, 278.6953125, 56.90625, 127.3125, 0.9133193492889404, 358.25, 431.484375, 0.982421875, 363.25, 426.328125, 0.96435546875, 352.0, 426.09375, 0.98095703125, 368.75, 428.671875, 0.52294921875, 341.25, 427.03125, 0.80078125, 378.75, 455.625, 0.97900390625, 323.5, 451.875, 0.98095703125, 391.0, 489.84375, 0.92578125, 296.25, 480.9375, 0.95361328125, 389.75, 520.3125, 0.90576171875, 300.0, 515.15625, 0.9375, 359.5, 524.53125, 0.9794921875, 325.25, 522.65625, 0.97998046875, 361.5, 581.25, 0.95068359375, 331.25, 577.96875, 0.955078125, 340.5, 625.3125, 0.89892578125, 316.0, 600.0, 0.90576171875]]</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 174.0, 277.53125, 59.5625, 128.625, 0.9128127098083496, 360.75, 428.203125, 0.9873046875, 365.75, 423.28125, 0.97216796875, 354.5, 423.046875, 0.9873046875, 371.0, 425.390625, 0.57421875, 343.5, 424.6875, 0.78076171875, 382.5, 453.75, 0.97509765625, 326.5, 448.359375, 0.97705078125, 398.5, 486.5625, 0.91552734375, 296.25, 469.921875, 0.92626953125, 392.0, 512.34375, 0.88623046875, 299.5, 502.5, 0.89892578125, 363.5, 524.0625, 0.97265625, 329.0, 521.71875, 0.97314453125, 363.0, 581.25, 0.93994140625, 335.25, 577.03125, 0.94140625, 344.0, 625.3125, 0.88818359375, 328.25, 618.75, 0.8896484375]]</t>
+          <t>[[0.0, 0.0, 173.984375, 277.53125, 59.46875, 128.625, 0.9128127098083496, 360.75, 428.203125, 0.98681640625, 365.75, 423.28125, 0.97216796875, 354.5, 423.046875, 0.9873046875, 371.0, 425.390625, 0.5751953125, 343.5, 424.6875, 0.78076171875, 382.5, 453.75, 0.97509765625, 326.5, 448.125, 0.97705078125, 398.5, 486.5625, 0.91552734375, 296.25, 469.921875, 0.92626953125, 392.0, 512.34375, 0.88623046875, 299.5, 502.5, 0.89892578125, 363.5, 524.0625, 0.97265625, 329.0, 521.71875, 0.97314453125, 363.0, 581.25, 0.93994140625, 335.25, 577.03125, 0.94189453125, 344.0, 625.3125, 0.88818359375, 328.25, 618.75, 0.89013671875]]</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 176.546875, 277.109375, 61.6875, 130.0, 0.9051604270935059, 360.0, 424.6875, 0.98193359375, 364.75, 419.0625, 0.96240234375, 353.75, 419.53125, 0.9765625, 370.75, 422.109375, 0.583984375, 343.0, 422.578125, 0.8017578125, 383.75, 450.0, 0.9794921875, 326.75, 445.3125, 0.97900390625, 405.25, 482.34375, 0.9287109375, 298.25, 463.828125, 0.94677734375, 398.5, 499.21875, 0.90771484375, 304.0, 496.875, 0.931640625, 365.5, 520.3125, 0.98046875, 331.25, 517.96875, 0.98046875, 365.0, 577.5, 0.95703125, 341.25, 569.0625, 0.9580078125, 344.0, 619.21875, 0.9111328125, 340.0, 614.53125, 0.9140625]]</t>
+          <t>[[0.0, 0.0, 176.5390625, 277.1171875, 61.6875, 130.0, 0.9051604270935059, 360.0, 424.6875, 0.98193359375, 364.75, 419.0625, 0.96240234375, 353.75, 419.53125, 0.9765625, 370.75, 422.109375, 0.58544921875, 343.0, 422.578125, 0.80126953125, 383.75, 450.0, 0.9794921875, 327.0, 445.3125, 0.97900390625, 405.25, 482.34375, 0.9287109375, 298.25, 463.828125, 0.94677734375, 398.5, 499.21875, 0.90771484375, 304.0, 496.875, 0.931640625, 365.5, 520.3125, 0.98046875, 331.25, 517.96875, 0.98046875, 365.0, 577.5, 0.95703125, 341.25, 569.0625, 0.9580078125, 344.0, 619.21875, 0.91162109375, 340.0, 614.53125, 0.9140625]]</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 178.84375, 274.9375, 63.03125, 132.75, 0.906090259552002, 361.75, 419.296875, 0.98779296875, 366.25, 413.90625, 0.97119140625, 355.0, 414.140625, 0.98779296875, 371.25, 415.78125, 0.55322265625, 343.5, 416.25, 0.79150390625, 387.5, 443.90625, 0.97607421875, 329.0, 440.859375, 0.9775390625, 410.0, 476.015625, 0.9189453125, 303.25, 458.671875, 0.9287109375, 393.25, 488.90625, 0.8916015625, 311.0, 486.5625, 0.90380859375, 370.25, 515.15625, 0.97412109375, 335.25, 513.28125, 0.974609375, 367.5, 574.6875, 0.9423828125, 346.75, 565.78125, 0.94482421875, 349.25, 619.21875, 0.8896484375, 347.0, 614.0625, 0.89306640625]]</t>
+          <t>[[0.0, 0.0, 178.875, 274.9375, 63.03125, 132.75, 0.906090259552002, 361.75, 419.0625, 0.98779296875, 366.25, 413.90625, 0.97119140625, 355.0, 414.140625, 0.98779296875, 371.25, 415.78125, 0.552734375, 343.5, 416.25, 0.79150390625, 387.5, 443.90625, 0.97607421875, 329.0, 440.859375, 0.9775390625, 410.0, 476.015625, 0.9189453125, 303.25, 458.671875, 0.9287109375, 393.25, 488.90625, 0.8916015625, 311.0, 486.5625, 0.90380859375, 370.25, 515.15625, 0.97412109375, 335.25, 513.28125, 0.974609375, 367.5, 574.6875, 0.9423828125, 346.75, 565.78125, 0.94482421875, 349.25, 619.21875, 0.8896484375, 347.0, 614.0625, 0.89306640625]]</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 180.921875, 274.6796875, 63.84375, 136.375, 0.9152390956878662, 361.25, 413.90625, 0.98095703125, 366.0, 408.515625, 0.96337890625, 355.25, 408.984375, 0.9755859375, 372.5, 411.09375, 0.60986328125, 343.25, 411.09375, 0.798828125, 387.0, 438.515625, 0.98095703125, 330.0, 436.875, 0.98046875, 414.5, 470.390625, 0.93994140625, 304.75, 454.921875, 0.953125, 391.75, 482.34375, 0.9248046875, 314.0, 483.28125, 0.94287109375, 376.0, 510.46875, 0.98388671875, 341.5, 509.0625, 0.9833984375, 368.5, 568.59375, 0.96533203125, 355.5, 563.4375, 0.96630859375, 347.0, 613.59375, 0.9248046875, 360.0, 617.8125, 0.9267578125]]</t>
+          <t>[[0.0, 0.0, 180.921875, 274.6796875, 63.84375, 136.125, 0.9152390956878662, 361.25, 413.90625, 0.98095703125, 366.0, 408.515625, 0.96337890625, 355.25, 408.984375, 0.9755859375, 372.5, 411.09375, 0.60986328125, 343.25, 411.09375, 0.798828125, 387.0, 438.515625, 0.98095703125, 330.0, 436.875, 0.98046875, 414.25, 470.390625, 0.93994140625, 304.75, 455.15625, 0.953125, 391.75, 482.34375, 0.9248046875, 314.0, 483.28125, 0.94287109375, 376.0, 510.46875, 0.98388671875, 341.5, 509.0625, 0.9833984375, 368.5, 568.59375, 0.96533203125, 355.5, 563.4375, 0.96630859375, 347.0, 613.59375, 0.9248046875, 360.0, 617.8125, 0.9267578125]]</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 182.71875, 275.4375, 64.9375, 143.875, 0.9214558601379395, 361.5, 408.75, 0.99072265625, 366.75, 403.59375, 0.97998046875, 354.5, 403.59375, 0.98876953125, 373.0, 405.9375, 0.669921875, 343.25, 406.171875, 0.78369140625, 390.5, 431.953125, 0.978515625, 330.0, 433.828125, 0.9794921875, 420.5, 465.703125, 0.9287109375, 308.75, 459.375, 0.93603515625, 392.25, 476.953125, 0.9072265625, 320.5, 486.09375, 0.9150390625, 382.5, 508.59375, 0.97998046875, 344.0, 508.59375, 0.98046875, 366.0, 566.71875, 0.96240234375, 361.0, 567.1875, 0.96435546875, 347.75, 609.84375, 0.93212890625, 373.0, 633.75, 0.9345703125]]</t>
+          <t>[[0.0, 0.0, 182.71875, 275.4375, 64.9375, 143.875, 0.9214558601379395, 361.5, 408.75, 0.99072265625, 366.75, 403.59375, 0.97998046875, 354.5, 403.59375, 0.98876953125, 373.0, 405.9375, 0.67041015625, 343.25, 406.171875, 0.78369140625, 390.5, 431.953125, 0.978515625, 330.0, 433.828125, 0.9794921875, 420.5, 465.703125, 0.9287109375, 308.75, 459.375, 0.93603515625, 392.25, 476.953125, 0.9072265625, 320.5, 486.09375, 0.9150390625, 382.5, 508.59375, 0.97998046875, 344.0, 508.59375, 0.98046875, 366.0, 566.71875, 0.96240234375, 361.0, 567.1875, 0.96435546875, 347.75, 609.84375, 0.93212890625, 373.0, 633.75, 0.93408203125]]</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 184.59375, 275.8125, 64.125, 147.75, 0.9233765602111816, 362.0, 406.40625, 0.9921875, 367.5, 400.78125, 0.984375, 355.0, 401.25, 0.990234375, 374.5, 404.0625, 0.71142578125, 343.5, 404.53125, 0.7880859375, 392.25, 430.3125, 0.9794921875, 330.5, 435.9375, 0.98046875, 424.0, 461.25, 0.931640625, 312.0, 467.578125, 0.93701171875, 396.25, 474.140625, 0.91064453125, 325.5, 496.40625, 0.91650390625, 387.75, 509.0625, 0.98046875, 350.5, 510.9375, 0.98095703125, 370.5, 568.125, 0.96337890625, 365.5, 570.9375, 0.96533203125, 352.5, 609.375, 0.9345703125, 377.0, 635.625, 0.9365234375]]</t>
+          <t>[[0.0, 0.0, 184.59375, 275.8125, 64.125, 147.75, 0.9228963851928711, 362.0, 406.40625, 0.9921875, 367.5, 400.78125, 0.984375, 355.0, 401.25, 0.990234375, 374.5, 404.0625, 0.71142578125, 343.5, 404.53125, 0.7880859375, 392.25, 430.3125, 0.9794921875, 330.5, 435.9375, 0.98046875, 424.0, 461.25, 0.931640625, 312.0, 467.578125, 0.93701171875, 396.25, 474.140625, 0.9111328125, 325.5, 496.40625, 0.91650390625, 387.75, 509.0625, 0.98046875, 350.5, 510.9375, 0.98095703125, 370.5, 568.125, 0.96337890625, 365.5, 570.9375, 0.96533203125, 352.5, 609.375, 0.9345703125, 377.0, 635.625, 0.9365234375]]</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 186.8515625, 275.8125, 63.3125, 149.875, 0.9224162101745605, 363.0, 405.46875, 0.99072265625, 368.75, 400.078125, 0.978515625, 356.0, 400.078125, 0.9853515625, 376.75, 403.828125, 0.68505859375, 344.75, 404.0625, 0.77783203125, 394.0, 430.78125, 0.9794921875, 332.5, 439.6875, 0.9765625, 427.0, 461.953125, 0.9326171875, 317.0, 476.015625, 0.92431640625, 400.5, 476.015625, 0.9072265625, 332.25, 501.5625, 0.9033203125, 393.0, 512.8125, 0.97802734375, 355.5, 516.09375, 0.9765625, 380.5, 575.625, 0.95556640625, 370.5, 576.5625, 0.95458984375, 354.5, 608.90625, 0.916015625, 380.5, 636.09375, 0.91357421875]]</t>
+          <t>[[0.0, 0.0, 186.8515625, 275.8125, 63.3125, 149.875, 0.9224162101745605, 363.0, 405.46875, 0.99072265625, 368.75, 400.078125, 0.978515625, 356.0, 400.078125, 0.9853515625, 376.5, 403.59375, 0.685546875, 344.75, 404.0625, 0.77783203125, 394.0, 430.78125, 0.9794921875, 332.5, 439.6875, 0.9765625, 427.0, 462.1875, 0.9326171875, 317.0, 476.015625, 0.92431640625, 400.5, 476.015625, 0.9072265625, 332.25, 501.5625, 0.9033203125, 393.0, 512.8125, 0.97802734375, 355.5, 516.09375, 0.9765625, 380.5, 575.625, 0.95556640625, 370.5, 576.5625, 0.95458984375, 354.5, 608.90625, 0.916015625, 380.5, 636.09375, 0.91357421875]]</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 188.4140625, 275.96875, 63.09375, 149.875, 0.9195351600646973, 364.5, 405.46875, 0.9892578125, 370.5, 400.078125, 0.97705078125, 357.75, 400.078125, 0.9833984375, 378.25, 404.296875, 0.70166015625, 347.0, 405.0, 0.7646484375, 397.0, 432.1875, 0.978515625, 336.0, 441.328125, 0.9755859375, 429.75, 464.296875, 0.93017578125, 321.0, 480.9375, 0.91796875, 403.0, 481.40625, 0.90283203125, 335.0, 506.25, 0.89453125, 397.25, 515.15625, 0.9765625, 360.0, 518.4375, 0.97509765625, 392.0, 582.1875, 0.94921875, 373.75, 578.4375, 0.947265625, 371.5, 617.8125, 0.89990234375, 383.25, 633.75, 0.89697265625]]</t>
+          <t>[[0.0, 0.0, 188.4140625, 275.96875, 63.09375, 149.875, 0.9195351600646973, 364.5, 405.234375, 0.9892578125, 370.5, 399.84375, 0.97705078125, 357.75, 400.078125, 0.9833984375, 378.25, 404.296875, 0.701171875, 347.0, 405.0, 0.7646484375, 397.0, 432.1875, 0.978515625, 336.0, 441.328125, 0.9755859375, 429.75, 464.296875, 0.93017578125, 321.0, 480.9375, 0.91796875, 403.0, 481.40625, 0.90283203125, 335.0, 506.25, 0.89453125, 397.25, 515.15625, 0.9765625, 360.0, 518.4375, 0.97509765625, 392.0, 582.1875, 0.94921875, 373.75, 578.4375, 0.947265625, 371.5, 617.8125, 0.89990234375, 383.25, 633.75, 0.89697265625]]</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 190.8828125, 276.46875, 61.5625, 151.125, 0.9233765602111816, 368.0, 405.234375, 0.98876953125, 373.25, 399.84375, 0.970703125, 360.5, 400.3125, 0.98486328125, 380.0, 404.0625, 0.599609375, 348.75, 405.46875, 0.77587890625, 399.5, 433.125, 0.978515625, 337.25, 442.734375, 0.9755859375, 433.0, 465.9375, 0.927734375, 328.5, 483.75, 0.9169921875, 409.5, 485.15625, 0.900390625, 338.0, 503.4375, 0.8935546875, 400.5, 516.5625, 0.9765625, 362.0, 520.3125, 0.97509765625, 401.75, 584.53125, 0.9501953125, 373.5, 585.0, 0.94873046875, 380.0, 609.84375, 0.90478515625, 383.75, 635.625, 0.90185546875]]</t>
+          <t>[[0.0, 0.0, 190.8828125, 276.46875, 61.5625, 151.125, 0.9233765602111816, 368.0, 405.234375, 0.98876953125, 373.25, 399.84375, 0.970703125, 360.75, 400.3125, 0.98486328125, 380.0, 404.0625, 0.59912109375, 348.75, 405.46875, 0.77587890625, 399.75, 433.125, 0.978515625, 337.25, 442.734375, 0.9755859375, 433.0, 465.9375, 0.927734375, 328.5, 483.75, 0.9169921875, 409.5, 485.15625, 0.900390625, 338.0, 503.4375, 0.8935546875, 400.5, 516.5625, 0.9765625, 362.0, 520.3125, 0.97509765625, 401.75, 584.53125, 0.9501953125, 373.5, 585.0, 0.94873046875, 380.0, 609.84375, 0.90478515625, 383.75, 636.09375, 0.90185546875]]</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 193.59375, 276.3125, 60.75, 151.5, 0.9209756851196289, 370.0, 404.53125, 0.98876953125, 375.5, 398.90625, 0.97216796875, 363.0, 399.140625, 0.98486328125, 383.0, 402.890625, 0.59619140625, 351.25, 404.0625, 0.75341796875, 403.5, 432.65625, 0.97802734375, 341.5, 443.4375, 0.9736328125, 438.5, 464.53125, 0.927734375, 335.5, 485.625, 0.904296875, 417.5, 485.15625, 0.89892578125, 343.5, 499.21875, 0.87744140625, 403.0, 518.90625, 0.9765625, 364.25, 523.59375, 0.9736328125, 404.25, 585.9375, 0.9501953125, 373.0, 589.6875, 0.94677734375, 386.5, 615.9375, 0.9072265625, 383.75, 637.03125, 0.9013671875]]</t>
+          <t>[[0.0, 0.0, 193.578125, 276.3125, 60.75, 151.5, 0.9209756851196289, 370.0, 404.53125, 0.98876953125, 375.5, 398.90625, 0.9716796875, 363.0, 399.140625, 0.98486328125, 383.0, 402.890625, 0.59619140625, 351.25, 404.0625, 0.75341796875, 403.5, 432.65625, 0.97802734375, 341.5, 443.4375, 0.9736328125, 438.5, 464.53125, 0.927734375, 335.5, 485.625, 0.904296875, 417.5, 485.15625, 0.89892578125, 343.5, 499.21875, 0.87744140625, 403.0, 518.90625, 0.9765625, 364.25, 523.59375, 0.9736328125, 404.25, 585.9375, 0.9501953125, 373.0, 589.6875, 0.94677734375, 386.5, 615.9375, 0.9072265625, 383.75, 637.03125, 0.9013671875]]</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 195.28125, 275.15625, 61.28125, 152.0, 0.9180946350097656, 374.5, 401.25, 0.990234375, 380.25, 395.859375, 0.9736328125, 367.5, 396.09375, 0.98828125, 387.25, 399.84375, 0.564453125, 355.25, 400.78125, 0.76318359375, 406.75, 429.84375, 0.97900390625, 344.5, 441.328125, 0.97509765625, 442.0, 461.953125, 0.92822265625, 342.0, 485.15625, 0.9091796875, 422.5, 482.8125, 0.900390625, 346.75, 487.5, 0.8828125, 406.5, 517.96875, 0.97705078125, 368.0, 523.59375, 0.97509765625, 407.0, 580.78125, 0.9521484375, 374.75, 587.8125, 0.94921875, 402.5, 617.8125, 0.91064453125, 382.75, 638.4375, 0.9052734375]]</t>
+          <t>[[0.0, 0.0, 195.296875, 275.15625, 61.28125, 152.0, 0.9180946350097656, 374.5, 401.25, 0.990234375, 380.25, 395.859375, 0.9736328125, 367.25, 396.09375, 0.98828125, 387.25, 399.84375, 0.5654296875, 355.25, 400.78125, 0.76318359375, 406.75, 429.84375, 0.97900390625, 344.5, 441.328125, 0.97509765625, 442.0, 461.953125, 0.92822265625, 342.0, 485.15625, 0.9091796875, 422.5, 482.8125, 0.900390625, 347.0, 487.5, 0.8828125, 406.5, 517.96875, 0.97705078125, 368.0, 523.59375, 0.97509765625, 407.0, 580.78125, 0.9521484375, 374.75, 587.8125, 0.94921875, 402.5, 617.34375, 0.91064453125, 382.75, 638.4375, 0.9052734375]]</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 196.546875, 274.0625, 62.0, 154.0, 0.9156937599182129, 378.0, 397.265625, 0.99072265625, 383.5, 391.640625, 0.97509765625, 370.75, 391.875, 0.98779296875, 390.75, 395.625, 0.59423828125, 359.5, 396.5625, 0.74560546875, 410.25, 426.09375, 0.9794921875, 350.25, 437.34375, 0.97705078125, 446.25, 459.140625, 0.9326171875, 344.25, 485.15625, 0.91943359375, 425.5, 479.765625, 0.9091796875, 343.75, 462.65625, 0.8974609375, 408.0, 513.75, 0.97802734375, 369.5, 518.90625, 0.9765625, 407.5, 575.625, 0.955078125, 374.5, 585.46875, 0.95263671875, 408.5, 627.1875, 0.91259765625, 384.25, 638.4375, 0.90771484375]]</t>
+          <t>[[0.0, 0.0, 196.546875, 274.0625, 62.0, 154.0, 0.9156937599182129, 377.75, 397.265625, 0.99072265625, 383.5, 391.640625, 0.97509765625, 370.5, 391.875, 0.98779296875, 390.75, 395.625, 0.5947265625, 359.5, 396.5625, 0.74560546875, 410.25, 426.09375, 0.9794921875, 350.25, 437.34375, 0.97705078125, 446.25, 459.140625, 0.9326171875, 344.25, 485.15625, 0.91943359375, 425.5, 479.765625, 0.9091796875, 343.75, 462.65625, 0.8974609375, 408.0, 513.75, 0.97802734375, 369.5, 518.90625, 0.9765625, 407.5, 575.625, 0.955078125, 374.5, 585.46875, 0.95263671875, 408.5, 627.1875, 0.91259765625, 384.25, 638.4375, 0.90771484375]]</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 198.25, 273.6875, 62.09375, 158.875, 0.9128127098083496, 384.25, 392.109375, 0.99169921875, 390.0, 386.71875, 0.97412109375, 376.75, 386.25, 0.990234375, 396.5, 390.9375, 0.5185546875, 364.75, 390.46875, 0.76025390625, 413.75, 421.875, 0.9794921875, 354.25, 429.84375, 0.97705078125, 450.0, 456.09375, 0.93212890625, 347.0, 475.3125, 0.9208984375, 429.0, 477.65625, 0.9091796875, 344.0, 445.546875, 0.8984375, 411.0, 509.0625, 0.97900390625, 372.5, 513.28125, 0.9775390625, 408.0, 573.28125, 0.95751953125, 375.5, 582.1875, 0.955078125, 410.0, 634.6875, 0.91552734375, 387.5, 638.4375, 0.9111328125]]</t>
+          <t>[[0.0, 0.0, 198.25, 273.6875, 62.09375, 158.875, 0.9123325347900391, 384.25, 392.109375, 0.99169921875, 390.0, 386.484375, 0.97412109375, 376.75, 386.25, 0.990234375, 396.5, 390.9375, 0.51904296875, 364.75, 390.46875, 0.76025390625, 413.75, 421.875, 0.9794921875, 354.25, 429.84375, 0.97705078125, 450.0, 456.09375, 0.93212890625, 347.0, 475.3125, 0.9208984375, 429.0, 477.65625, 0.90869140625, 344.0, 445.546875, 0.8984375, 411.0, 509.0625, 0.97900390625, 372.5, 513.28125, 0.9775390625, 408.0, 573.28125, 0.95751953125, 375.5, 582.1875, 0.955078125, 410.0, 634.6875, 0.91552734375, 387.5, 638.4375, 0.9111328125]]</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 199.484375, 273.78125, 62.0, 163.625, 0.9132928848266602, 387.5, 386.71875, 0.9921875, 393.5, 381.5625, 0.9794921875, 380.5, 381.09375, 0.98974609375, 400.25, 386.484375, 0.615234375, 369.75, 385.78125, 0.73046875, 417.5, 417.65625, 0.97900390625, 359.5, 420.46875, 0.97705078125, 451.25, 453.984375, 0.93310546875, 348.5, 459.609375, 0.9228515625, 431.5, 477.890625, 0.91064453125, 346.5, 422.578125, 0.9013671875, 414.0, 506.71875, 0.97998046875, 376.0, 508.125, 0.978515625, 411.75, 574.21875, 0.9609375, 378.5, 577.03125, 0.95849609375, 411.0, 640.3125, 0.9228515625, 384.75, 634.21875, 0.91943359375]]</t>
+          <t>[[0.0, 0.0, 199.484375, 273.78125, 62.09375, 163.625, 0.9132928848266602, 387.5, 386.71875, 0.9921875, 393.5, 381.5625, 0.9794921875, 380.5, 381.09375, 0.98974609375, 400.25, 386.484375, 0.615234375, 369.75, 385.78125, 0.73046875, 417.5, 417.65625, 0.97900390625, 359.5, 420.46875, 0.97705078125, 451.25, 453.984375, 0.93310546875, 348.5, 459.609375, 0.9228515625, 431.5, 477.890625, 0.91064453125, 346.5, 422.578125, 0.9013671875, 414.0, 506.71875, 0.97998046875, 376.0, 508.125, 0.978515625, 411.75, 574.21875, 0.9609375, 378.5, 577.03125, 0.95849609375, 411.0, 640.3125, 0.9228515625, 384.75, 634.21875, 0.91943359375]]</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 199.265625, 274.5, 65.125, 169.625, 0.9156937599182129, 392.25, 383.90625, 0.9912109375, 398.25, 378.984375, 0.9794921875, 385.25, 378.515625, 0.9873046875, 405.0, 383.90625, 0.65966796875, 373.75, 382.96875, 0.7431640625, 421.25, 416.25, 0.97900390625, 363.25, 416.71875, 0.97705078125, 453.75, 453.046875, 0.9345703125, 344.0, 435.46875, 0.92724609375, 434.0, 477.890625, 0.9140625, 344.25, 394.921875, 0.908203125, 416.5, 507.1875, 0.98046875, 378.25, 508.125, 0.9794921875, 414.5, 575.625, 0.96142578125, 382.0, 577.5, 0.95947265625, 410.25, 645.0, 0.9208984375, 387.5, 634.6875, 0.91748046875]]</t>
+          <t>[[0.0, 0.0, 199.25, 274.5, 65.125, 169.625, 0.9156937599182129, 392.25, 383.90625, 0.9912109375, 398.25, 378.984375, 0.9794921875, 385.25, 378.515625, 0.9873046875, 405.0, 383.90625, 0.66015625, 373.75, 382.96875, 0.74365234375, 421.25, 416.25, 0.97900390625, 363.25, 416.71875, 0.97705078125, 453.75, 453.046875, 0.9345703125, 344.0, 435.46875, 0.92724609375, 434.0, 477.890625, 0.9140625, 344.25, 394.921875, 0.908203125, 416.5, 507.1875, 0.98046875, 378.25, 508.125, 0.9794921875, 414.5, 575.625, 0.96142578125, 382.0, 577.5, 0.95947265625, 410.25, 645.0, 0.9208984375, 387.5, 634.6875, 0.91748046875]]</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 199.140625, 273.3125, 68.4375, 175.875, 0.9152135848999023, 397.0, 382.734375, 0.9921875, 404.25, 377.34375, 0.9853515625, 389.75, 376.875, 0.9873046875, 412.25, 383.203125, 0.759765625, 378.0, 382.5, 0.73974609375, 426.5, 416.71875, 0.978515625, 368.25, 413.4375, 0.97705078125, 456.75, 454.6875, 0.935546875, 344.0, 412.96875, 0.9296875, 437.25, 477.890625, 0.91650390625, 343.25, 372.421875, 0.912109375, 419.5, 509.0625, 0.98095703125, 380.75, 509.0625, 0.97998046875, 417.5, 579.84375, 0.96142578125, 384.0, 579.375, 0.95947265625, 408.5, 647.8125, 0.92041015625, 392.5, 621.5625, 0.9169921875]]</t>
+          <t>[[0.0, 0.0, 199.125, 273.3125, 68.4375, 175.875, 0.9152135848999023, 397.0, 382.734375, 0.9921875, 404.25, 377.34375, 0.9853515625, 389.75, 376.875, 0.9873046875, 412.25, 383.203125, 0.759765625, 378.0, 382.5, 0.73974609375, 426.5, 416.71875, 0.978515625, 368.25, 413.4375, 0.97705078125, 456.75, 454.6875, 0.935546875, 344.0, 412.96875, 0.9296875, 437.25, 477.890625, 0.91650390625, 343.5, 372.421875, 0.912109375, 419.5, 509.0625, 0.98095703125, 380.75, 509.0625, 0.97998046875, 417.5, 579.84375, 0.96142578125, 384.0, 579.375, 0.95947265625, 408.5, 647.8125, 0.92041015625, 392.5, 621.5625, 0.9169921875]]</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 200.140625, 269.828125, 70.3125, 187.0, 0.9200153350830078, 402.25, 384.375, 0.9873046875, 409.25, 378.75, 0.97998046875, 395.0, 378.515625, 0.9755859375, 418.25, 384.609375, 0.79248046875, 384.0, 385.3125, 0.7080078125, 433.25, 419.53125, 0.978515625, 372.0, 413.203125, 0.97705078125, 460.25, 459.609375, 0.93994140625, 344.75, 392.109375, 0.93212890625, 438.0, 480.46875, 0.92431640625, 345.5, 349.921875, 0.91650390625, 422.5, 512.34375, 0.9814453125, 382.0, 510.9375, 0.98095703125, 420.25, 583.59375, 0.962890625, 381.75, 580.3125, 0.9599609375, 410.25, 652.5, 0.921875, 393.5, 609.84375, 0.91796875]]</t>
+          <t>[[0.0, 0.0, 200.140625, 269.828125, 70.3125, 187.0, 0.9200153350830078, 402.25, 384.375, 0.9873046875, 409.25, 378.75, 0.98046875, 395.0, 378.515625, 0.9755859375, 418.25, 384.375, 0.79296875, 384.0, 385.3125, 0.7080078125, 433.25, 419.53125, 0.978515625, 372.0, 413.203125, 0.97705078125, 460.25, 459.609375, 0.93994140625, 344.75, 392.109375, 0.93212890625, 438.0, 480.46875, 0.92431640625, 345.5, 349.921875, 0.91650390625, 422.5, 512.34375, 0.9814453125, 382.0, 510.9375, 0.98095703125, 420.25, 583.59375, 0.962890625, 381.75, 580.3125, 0.9599609375, 410.25, 652.5, 0.921875, 393.5, 609.84375, 0.91796875]]</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 201.609375, 269.125, 71.0, 190.5, 0.9252972602844238, 408.75, 386.953125, 0.9853515625, 416.0, 381.328125, 0.9775390625, 402.25, 380.625, 0.9716796875, 425.0, 386.71875, 0.78369140625, 391.0, 385.3125, 0.70654296875, 439.0, 424.921875, 0.978515625, 376.0, 414.375, 0.9775390625, 464.5, 463.828125, 0.94189453125, 345.25, 386.953125, 0.93505859375, 437.5, 483.28125, 0.92724609375, 349.5, 345.0, 0.92041015625, 425.75, 516.09375, 0.9814453125, 384.75, 512.8125, 0.98095703125, 423.25, 589.21875, 0.9619140625, 384.25, 582.1875, 0.958984375, 410.5, 657.1875, 0.91796875, 393.5, 601.875, 0.9140625]]</t>
+          <t>[[0.0, 0.0, 201.609375, 269.140625, 71.0, 190.5, 0.9252972602844238, 408.75, 386.953125, 0.9853515625, 416.0, 381.328125, 0.9775390625, 402.25, 380.390625, 0.9716796875, 425.0, 386.71875, 0.78369140625, 391.0, 385.3125, 0.70703125, 439.0, 424.921875, 0.978515625, 376.0, 414.375, 0.9775390625, 464.5, 463.828125, 0.94189453125, 345.25, 386.953125, 0.93505859375, 437.5, 483.28125, 0.92724609375, 349.5, 345.0, 0.92041015625, 425.75, 516.09375, 0.9814453125, 384.75, 512.8125, 0.98095703125, 423.25, 589.21875, 0.9619140625, 384.25, 582.1875, 0.958984375, 410.5, 657.1875, 0.91796875, 393.5, 601.875, 0.9140625]]</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 202.0625, 272.3125, 72.3125, 184.5, 0.9252972602844238, 414.75, 388.59375, 0.98974609375, 422.5, 383.4375, 0.98486328125, 408.0, 382.03125, 0.9814453125, 431.25, 389.296875, 0.8134765625, 396.0, 386.484375, 0.7265625, 443.5, 427.96875, 0.978515625, 379.25, 417.1875, 0.97802734375, 467.0, 464.296875, 0.9404296875, 344.5, 387.65625, 0.9365234375, 439.0, 477.65625, 0.92724609375, 359.25, 353.671875, 0.9228515625, 429.5, 518.90625, 0.98095703125, 388.5, 515.15625, 0.98095703125, 427.75, 593.4375, 0.96044921875, 391.5, 584.0625, 0.95751953125, 411.25, 660.46875, 0.912109375, 392.5, 596.71875, 0.9091796875]]</t>
+          <t>[[0.0, 0.0, 202.0625, 272.3125, 72.3125, 184.5, 0.9252972602844238, 414.75, 388.59375, 0.98974609375, 422.5, 383.4375, 0.98486328125, 408.0, 382.03125, 0.9814453125, 431.25, 389.296875, 0.8134765625, 396.0, 386.484375, 0.72705078125, 443.5, 427.734375, 0.978515625, 379.25, 417.1875, 0.97802734375, 467.0, 464.296875, 0.9404296875, 344.5, 387.65625, 0.9365234375, 439.0, 477.65625, 0.92724609375, 359.25, 353.671875, 0.9228515625, 429.5, 518.90625, 0.98095703125, 388.5, 515.15625, 0.98095703125, 427.75, 593.4375, 0.9599609375, 391.5, 584.0625, 0.95751953125, 411.25, 660.46875, 0.912109375, 392.5, 596.71875, 0.9091796875]]</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 202.546875, 276.875, 73.125, 173.75, 0.9300990104675293, 420.25, 387.421875, 0.9912109375, 427.5, 382.5, 0.9873046875, 414.0, 381.328125, 0.98046875, 436.5, 388.59375, 0.857421875, 403.5, 385.546875, 0.70263671875, 448.0, 426.5625, 0.97705078125, 383.75, 416.953125, 0.97705078125, 468.5, 460.78125, 0.93701171875, 342.5, 386.015625, 0.93359375, 438.0, 462.65625, 0.923828125, 377.25, 372.890625, 0.9189453125, 432.5, 519.84375, 0.98046875, 392.0, 515.625, 0.97998046875, 431.0, 593.90625, 0.95947265625, 401.0, 577.96875, 0.95703125, 411.0, 660.46875, 0.91357421875, 391.5, 595.3125, 0.91162109375]]</t>
+          <t>[[0.0, 0.0, 202.5625, 276.84375, 73.125, 173.75, 0.9300990104675293, 420.25, 387.421875, 0.9912109375, 427.5, 382.5, 0.9873046875, 414.0, 381.328125, 0.98046875, 436.5, 388.59375, 0.85791015625, 403.5, 385.546875, 0.70263671875, 448.0, 426.5625, 0.97705078125, 383.75, 416.953125, 0.97705078125, 468.5, 460.78125, 0.93701171875, 342.5, 386.015625, 0.93359375, 438.0, 462.65625, 0.923828125, 377.5, 372.65625, 0.9189453125, 432.5, 519.84375, 0.98046875, 392.0, 515.625, 0.97998046875, 431.0, 593.90625, 0.95947265625, 401.0, 577.96875, 0.95703125, 411.0, 660.46875, 0.91357421875, 391.5, 595.3125, 0.91162109375]]</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 202.9375, 276.53125, 73.8125, 173.25, 0.9267377853393555, 425.5, 384.140625, 0.99365234375, 433.5, 380.15625, 0.98876953125, 420.25, 377.8125, 0.9873046875, 442.0, 387.421875, 0.8203125, 408.25, 380.625, 0.72900390625, 452.5, 421.640625, 0.9755859375, 387.5, 409.6875, 0.9765625, 471.5, 447.1875, 0.93115234375, 344.75, 382.03125, 0.93408203125, 430.5, 440.625, 0.91748046875, 384.5, 389.296875, 0.919921875, 437.0, 513.75, 0.9794921875, 396.5, 505.78125, 0.9794921875, 434.0, 590.625, 0.9599609375, 411.25, 553.125, 0.958984375, 412.0, 658.125, 0.91796875, 395.5, 594.375, 0.92041015625]]</t>
+          <t>[[0.0, 0.0, 202.9375, 276.53125, 73.875, 173.25, 0.9267377853393555, 425.5, 384.140625, 0.99365234375, 433.5, 380.15625, 0.98876953125, 420.25, 377.8125, 0.9873046875, 442.0, 387.1875, 0.82080078125, 408.25, 380.625, 0.7294921875, 452.5, 421.640625, 0.9755859375, 387.5, 409.6875, 0.9765625, 471.5, 447.1875, 0.93115234375, 344.75, 382.03125, 0.93408203125, 430.5, 440.625, 0.91748046875, 384.5, 389.296875, 0.919921875, 437.0, 513.75, 0.9794921875, 396.5, 505.78125, 0.9794921875, 434.0, 590.625, 0.9599609375, 411.25, 553.125, 0.958984375, 412.0, 658.125, 0.91796875, 395.5, 594.375, 0.92041015625]]</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 203.4375, 274.59375, 72.9375, 178.25, 0.9137730598449707, 431.25, 375.9375, 0.9921875, 439.5, 372.1875, 0.982421875, 425.25, 369.609375, 0.98779296875, 447.25, 380.15625, 0.6865234375, 412.0, 374.0625, 0.73486328125, 456.5, 411.796875, 0.97314453125, 392.5, 403.359375, 0.97509765625, 471.5, 425.15625, 0.92724609375, 346.0, 382.96875, 0.93212890625, 430.0, 419.296875, 0.91357421875, 385.75, 394.453125, 0.91650390625, 443.0, 505.3125, 0.9775390625, 401.75, 498.75, 0.97802734375, 433.0, 583.125, 0.9560546875, 421.75, 537.1875, 0.9560546875, 411.5, 658.59375, 0.91015625, 404.75, 606.5625, 0.91455078125]]</t>
+          <t>[[0.0, 0.0, 203.421875, 274.59375, 72.9375, 178.25, 0.9137730598449707, 431.25, 375.9375, 0.9921875, 439.5, 372.1875, 0.982421875, 425.5, 369.609375, 0.98779296875, 447.25, 380.15625, 0.68701171875, 412.0, 374.0625, 0.73486328125, 456.5, 411.796875, 0.97314453125, 392.5, 403.359375, 0.97509765625, 471.5, 425.15625, 0.92724609375, 346.0, 382.96875, 0.93212890625, 430.0, 419.296875, 0.91357421875, 385.75, 394.453125, 0.91650390625, 443.0, 505.3125, 0.9775390625, 401.75, 498.75, 0.97802734375, 433.0, 583.125, 0.9560546875, 421.75, 537.1875, 0.9560546875, 411.5, 658.59375, 0.91015625, 404.75, 606.5625, 0.91455078125]]</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 203.296875, 272.75, 71.0, 180.875, 0.9046497344970703, 436.0, 368.671875, 0.9892578125, 444.5, 364.6875, 0.974609375, 430.5, 362.34375, 0.98046875, 453.0, 372.65625, 0.64501953125, 417.75, 365.859375, 0.69873046875, 460.0, 402.1875, 0.9677734375, 396.75, 396.09375, 0.9716796875, 466.25, 403.59375, 0.9150390625, 346.0, 380.625, 0.9267578125, 422.5, 396.5625, 0.89794921875, 390.0, 370.078125, 0.9072265625, 450.25, 497.8125, 0.97314453125, 410.0, 490.78125, 0.974609375, 433.75, 579.84375, 0.94384765625, 427.5, 526.875, 0.94482421875, 413.0, 657.1875, 0.8857421875, 418.0, 596.25, 0.892578125]]</t>
+          <t>[[0.0, 0.0, 203.296875, 272.75, 71.0, 180.875, 0.9046497344970703, 436.0, 368.671875, 0.9892578125, 444.5, 364.6875, 0.974609375, 430.5, 362.34375, 0.98046875, 453.0, 372.65625, 0.64599609375, 417.75, 365.859375, 0.69873046875, 460.0, 402.1875, 0.9677734375, 396.75, 396.09375, 0.9716796875, 466.25, 403.59375, 0.9150390625, 346.0, 380.625, 0.9267578125, 422.5, 396.5625, 0.89794921875, 390.0, 370.078125, 0.9072265625, 450.25, 497.8125, 0.97314453125, 410.0, 490.78125, 0.974609375, 433.75, 579.84375, 0.94384765625, 427.5, 526.875, 0.94482421875, 413.0, 657.1875, 0.88525390625, 418.0, 596.71875, 0.892578125]]</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 205.75, 267.71875, 68.375, 185.75, 0.8931255340576172, 441.0, 360.9375, 0.98974609375, 449.5, 356.484375, 0.97998046875, 435.5, 354.140625, 0.978515625, 459.5, 363.984375, 0.73193359375, 425.0, 356.71875, 0.5908203125, 467.5, 385.78125, 0.9638671875, 407.25, 386.953125, 0.97119140625, 445.5, 387.65625, 0.9033203125, 357.0, 380.15625, 0.92724609375, 411.75, 374.765625, 0.880859375, 388.5, 349.453125, 0.90478515625, 457.5, 485.625, 0.97509765625, 417.0, 483.28125, 0.9775390625, 442.75, 558.75, 0.9560546875, 425.5, 529.6875, 0.95947265625, 419.0, 635.15625, 0.9208984375, 433.75, 607.5, 0.927734375]]</t>
+          <t>[[0.0, 0.0, 205.75, 267.71875, 68.375, 185.75, 0.8931255340576172, 441.0, 360.9375, 0.98974609375, 449.5, 356.484375, 0.97998046875, 435.5, 354.140625, 0.978515625, 459.5, 363.984375, 0.732421875, 425.0, 356.71875, 0.59033203125, 467.5, 385.78125, 0.9638671875, 407.25, 386.953125, 0.97119140625, 445.5, 387.65625, 0.9033203125, 357.0, 380.15625, 0.92724609375, 411.5, 374.765625, 0.88134765625, 388.5, 349.453125, 0.90478515625, 457.5, 485.625, 0.97509765625, 417.0, 483.28125, 0.9775390625, 442.75, 558.75, 0.9560546875, 425.75, 529.6875, 0.95947265625, 419.25, 635.15625, 0.9208984375, 433.75, 607.5, 0.927734375]]</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 211.40625, 259.28125, 64.25, 190.5, 0.9233765602111816, 444.25, 350.625, 0.96044921875, 452.5, 345.9375, 0.91796875, 438.75, 344.0625, 0.91015625, 462.25, 355.078125, 0.59619140625, 428.0, 349.921875, 0.62890625, 467.5, 378.515625, 0.966796875, 415.0, 381.796875, 0.97607421875, 430.5, 367.96875, 0.896484375, 368.5, 376.875, 0.93310546875, 404.0, 346.40625, 0.87255859375, 388.0, 335.625, 0.91162109375, 464.25, 480.46875, 0.978515625, 425.0, 479.765625, 0.9814453125, 453.5, 555.0, 0.9658203125, 426.25, 541.875, 0.97021484375, 429.25, 622.5, 0.94091796875, 444.5, 615.0, 0.947265625]]</t>
+          <t>[[0.0, 0.0, 211.40625, 259.28125, 64.25, 190.5, 0.9233765602111816, 444.25, 350.625, 0.96044921875, 452.5, 345.9375, 0.91796875, 438.75, 344.296875, 0.90966796875, 462.25, 355.078125, 0.5966796875, 428.0, 349.921875, 0.62890625, 467.5, 378.515625, 0.966796875, 415.0, 381.796875, 0.97607421875, 430.5, 367.96875, 0.896484375, 368.5, 376.875, 0.93310546875, 404.0, 346.40625, 0.87255859375, 388.0, 335.625, 0.91162109375, 464.25, 480.46875, 0.978515625, 425.0, 479.765625, 0.9814453125, 453.5, 555.0, 0.9658203125, 426.25, 541.875, 0.97021484375, 429.25, 622.5, 0.94091796875, 444.25, 615.0, 0.947265625]]</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 217.15625, 255.3125, 59.5625, 191.125, 0.9161739349365234, 445.75, 345.703125, 0.93896484375, 453.75, 340.546875, 0.9208984375, 441.5, 339.609375, 0.79541015625, 467.5, 347.34375, 0.78955078125, 434.75, 344.296875, 0.41259765625, 471.0, 371.71875, 0.9599609375, 426.0, 375.703125, 0.97021484375, 416.5, 363.046875, 0.896484375, 386.25, 377.109375, 0.92041015625, 406.75, 331.875, 0.87060546875, 399.75, 332.8125, 0.89501953125, 471.0, 478.359375, 0.97607421875, 433.25, 478.125, 0.9794921875, 460.0, 557.8125, 0.96044921875, 429.75, 550.3125, 0.96435546875, 446.5, 604.6875, 0.92822265625, 448.75, 631.875, 0.9345703125]]</t>
+          <t>[[0.0, 0.0, 217.15625, 255.3125, 59.5625, 191.125, 0.9161739349365234, 445.75, 345.703125, 0.939453125, 453.75, 340.546875, 0.92138671875, 441.5, 339.609375, 0.79638671875, 467.5, 347.34375, 0.7900390625, 434.75, 344.296875, 0.41357421875, 471.0, 371.71875, 0.96044921875, 426.0, 375.703125, 0.97021484375, 416.5, 363.046875, 0.89599609375, 386.25, 377.109375, 0.92041015625, 406.75, 331.875, 0.87060546875, 399.75, 332.578125, 0.89501953125, 471.0, 478.359375, 0.97607421875, 433.0, 478.125, 0.9794921875, 460.0, 557.8125, 0.96044921875, 429.75, 550.3125, 0.96435546875, 446.5, 604.6875, 0.92822265625, 448.75, 631.875, 0.9345703125]]</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 222.65625, 261.359375, 56.9375, 189.25, 0.9041695594787598, 452.75, 349.453125, 0.87060546875, 459.0, 343.828125, 0.849609375, 448.5, 343.359375, 0.6416015625, 471.5, 347.109375, 0.75, 442.75, 346.640625, 0.33251953125, 481.0, 376.640625, 0.94677734375, 428.5, 380.625, 0.9560546875, 460.0, 357.1875, 0.908203125, 399.5, 381.09375, 0.91064453125, 426.5, 338.90625, 0.88720703125, 407.25, 345.0, 0.88330078125, 476.25, 481.875, 0.9755859375, 437.0, 483.28125, 0.97802734375, 461.75, 556.875, 0.9560546875, 430.75, 557.8125, 0.95751953125, 463.0, 615.9375, 0.916015625, 454.5, 632.8125, 0.9189453125]]</t>
+          <t>[[0.0, 0.0, 222.65625, 261.34375, 56.9375, 189.25, 0.9041695594787598, 452.75, 349.21875, 0.87060546875, 459.0, 343.828125, 0.84912109375, 448.5, 343.359375, 0.6416015625, 471.5, 347.109375, 0.7490234375, 442.75, 346.640625, 0.33349609375, 481.0, 376.640625, 0.94677734375, 428.5, 380.625, 0.9560546875, 460.0, 357.1875, 0.908203125, 399.5, 381.09375, 0.91064453125, 426.5, 338.90625, 0.88720703125, 407.25, 345.0, 0.88330078125, 476.25, 481.875, 0.9755859375, 437.0, 483.28125, 0.97802734375, 461.75, 556.875, 0.9560546875, 430.75, 557.8125, 0.95751953125, 463.0, 615.9375, 0.916015625, 454.5, 632.8125, 0.9189453125]]</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 228.25, 265.609375, 52.0, 191.375, 0.9013209342956543, 447.5, 355.78125, 0.869140625, 455.5, 348.984375, 0.9072265625, 443.0, 348.75, 0.654296875, 471.5, 350.625, 0.81396484375, 436.75, 351.5625, 0.21337890625, 484.0, 374.53125, 0.958984375, 431.0, 379.921875, 0.939453125, 464.0, 346.875, 0.93701171875, 416.5, 390.0, 0.82958984375, 429.25, 335.15625, 0.91552734375, 421.5, 355.78125, 0.81103515625, 482.25, 480.46875, 0.9833984375, 441.25, 482.34375, 0.97900390625, 464.5, 553.59375, 0.97216796875, 436.0, 569.53125, 0.96142578125, 480.5, 605.625, 0.93701171875, 457.0, 641.71875, 0.91796875]]</t>
+          <t>[[0.0, 0.0, 228.2421875, 265.609375, 52.03125, 191.375, 0.9013209342956543, 447.5, 355.78125, 0.86962890625, 455.5, 348.984375, 0.90771484375, 443.0, 348.75, 0.654296875, 471.5, 350.625, 0.814453125, 436.75, 351.5625, 0.21337890625, 484.0, 374.53125, 0.958984375, 431.0, 379.921875, 0.939453125, 464.0, 346.875, 0.93701171875, 416.5, 390.0, 0.82958984375, 429.25, 335.390625, 0.916015625, 421.5, 355.78125, 0.8115234375, 482.25, 480.46875, 0.9833984375, 441.25, 482.34375, 0.97900390625, 464.5, 553.59375, 0.97216796875, 436.0, 569.53125, 0.9619140625, 480.5, 605.625, 0.93701171875, 457.0, 641.71875, 0.91796875]]</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 231.4296875, 265.109375, 54.25, 206.0, 0.9051604270935059, 457.0, 361.875, 0.94287109375, 464.25, 354.84375, 0.9521484375, 452.0, 354.609375, 0.83740234375, 477.75, 355.78125, 0.810546875, 449.75, 357.65625, 0.266845703125, 491.0, 379.453125, 0.96826171875, 442.5, 390.0, 0.95947265625, 475.25, 341.25, 0.947265625, 430.5, 408.984375, 0.88525390625, 435.0, 319.6875, 0.93359375, 420.0, 396.5625, 0.87158203125, 490.0, 482.8125, 0.98583984375, 451.75, 487.5, 0.9833984375, 470.0, 546.09375, 0.97705078125, 441.25, 579.375, 0.97021484375, 496.5, 610.3125, 0.9453125, 463.75, 654.84375, 0.93115234375]]</t>
+          <t>[[0.0, 0.0, 231.4296875, 265.09375, 54.25, 206.0, 0.9046804904937744, 457.0, 361.875, 0.943359375, 464.25, 354.84375, 0.9521484375, 452.0, 354.609375, 0.83740234375, 477.75, 355.78125, 0.81103515625, 449.75, 357.65625, 0.266845703125, 491.0, 379.453125, 0.96826171875, 442.5, 390.0, 0.95947265625, 475.25, 341.484375, 0.947265625, 430.5, 408.984375, 0.88525390625, 435.0, 319.6875, 0.93359375, 420.0, 396.5625, 0.87158203125, 490.0, 482.8125, 0.98583984375, 451.75, 487.5, 0.9833984375, 470.0, 546.09375, 0.97705078125, 441.25, 579.375, 0.97021484375, 496.5, 610.3125, 0.9453125, 463.75, 654.84375, 0.93115234375]]</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 235.375, 262.28125, 54.28125, 233.125, 0.907050609588623, 471.5, 357.65625, 0.9306640625, 478.0, 352.265625, 0.83837890625, 465.5, 351.5625, 0.8662109375, 486.0, 356.484375, 0.401123046875, 452.5, 355.3125, 0.6201171875, 493.25, 387.1875, 0.96630859375, 437.25, 395.625, 0.96630859375, 488.5, 343.125, 0.9375, 428.0, 408.75, 0.921875, 446.0, 311.25, 0.9267578125, 444.25, 424.21875, 0.91162109375, 500.5, 487.96875, 0.98046875, 460.0, 494.53125, 0.97998046875, 478.25, 552.1875, 0.96875, 455.75, 586.875, 0.9677734375, 509.5, 621.5625, 0.9404296875, 473.25, 675.9375, 0.93603515625]]</t>
+          <t>[[0.0, 0.0, 235.375, 262.28125, 54.28125, 233.125, 0.9065704345703125, 471.5, 357.65625, 0.93017578125, 478.0, 352.265625, 0.83837890625, 465.25, 351.5625, 0.86572265625, 486.0, 356.484375, 0.4013671875, 452.5, 355.078125, 0.6201171875, 493.25, 387.1875, 0.96630859375, 437.25, 395.625, 0.96630859375, 488.5, 343.125, 0.9375, 428.0, 408.75, 0.921875, 446.0, 311.25, 0.9267578125, 444.25, 424.21875, 0.91162109375, 500.5, 488.4375, 0.98046875, 460.0, 494.53125, 0.97998046875, 478.0, 552.1875, 0.96875, 455.75, 586.875, 0.9677734375, 509.5, 621.5625, 0.9404296875, 473.25, 675.9375, 0.93603515625]]</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 238.703125, 260.28125, 56.3125, 236.125, 0.9089713096618652, 479.5, 366.09375, 0.94140625, 485.5, 360.46875, 0.81396484375, 472.0, 359.765625, 0.9130859375, 492.5, 364.6875, 0.2626953125, 456.25, 362.578125, 0.7138671875, 499.0, 396.09375, 0.9716796875, 438.5, 408.515625, 0.97265625, 499.25, 347.8125, 0.93701171875, 445.0, 446.71875, 0.92919921875, 466.5, 305.859375, 0.923828125, 447.75, 477.65625, 0.91357421875, 511.5, 495.0, 0.9814453125, 469.75, 502.96875, 0.9814453125, 490.25, 560.15625, 0.97021484375, 467.75, 594.375, 0.97021484375, 515.0, 643.125, 0.94287109375, 483.25, 680.15625, 0.939453125]]</t>
+          <t>[[0.0, 0.0, 238.703125, 260.28125, 56.40625, 236.125, 0.9089713096618652, 479.5, 366.09375, 0.94140625, 485.5, 360.46875, 0.81396484375, 472.0, 359.765625, 0.9130859375, 492.5, 364.6875, 0.262451171875, 456.25, 362.578125, 0.71435546875, 499.0, 396.09375, 0.9716796875, 438.5, 408.515625, 0.97265625, 499.25, 347.578125, 0.93701171875, 445.0, 446.71875, 0.92919921875, 466.5, 305.859375, 0.923828125, 447.75, 477.65625, 0.91357421875, 511.5, 495.0, 0.9814453125, 469.75, 502.96875, 0.9814453125, 490.25, 559.6875, 0.97021484375, 467.75, 594.375, 0.97021484375, 515.0, 643.125, 0.94287109375, 483.25, 680.15625, 0.939453125]]</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 242.1875, 259.6875, 57.125, 237.25, 0.8950462341308594, 482.0, 372.890625, 0.97216796875, 489.5, 367.5, 0.9189453125, 475.0, 365.859375, 0.95556640625, 497.25, 375.46875, 0.37548828125, 460.75, 371.015625, 0.66943359375, 505.0, 403.125, 0.9716796875, 445.0, 420.703125, 0.97412109375, 514.0, 352.96875, 0.9345703125, 451.5, 474.140625, 0.92919921875, 488.0, 302.8125, 0.91748046875, 446.25, 516.09375, 0.90966796875, 519.0, 505.78125, 0.98046875, 477.25, 514.6875, 0.98095703125, 504.0, 571.875, 0.9677734375, 470.75, 596.71875, 0.96826171875, 517.5, 661.875, 0.9365234375, 493.5, 674.0625, 0.935546875]]</t>
+          <t>[[0.0, 0.0, 242.1875, 259.671875, 57.125, 237.25, 0.8950462341308594, 482.0, 372.890625, 0.97216796875, 489.5, 367.5, 0.91845703125, 475.0, 365.859375, 0.95556640625, 497.25, 375.46875, 0.375244140625, 460.75, 371.015625, 0.66943359375, 505.0, 403.125, 0.9716796875, 445.0, 420.703125, 0.97412109375, 514.0, 352.96875, 0.9345703125, 451.5, 474.140625, 0.92919921875, 488.0, 302.8125, 0.91748046875, 446.5, 516.09375, 0.90966796875, 519.0, 505.78125, 0.98046875, 477.25, 514.6875, 0.98095703125, 504.0, 571.875, 0.9677734375, 470.75, 596.25, 0.96826171875, 517.5, 661.875, 0.9365234375, 493.5, 674.0625, 0.935546875]]</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 244.5625, 262.53125, 63.84375, 231.5, 0.9214558601379395, 488.0, 378.28125, 0.98876953125, 497.75, 373.828125, 0.974609375, 481.0, 370.78125, 0.97607421875, 507.75, 384.609375, 0.65234375, 467.25, 375.9375, 0.68798828125, 513.0, 409.453125, 0.97607421875, 452.75, 428.203125, 0.97900390625, 525.5, 370.78125, 0.93603515625, 451.5, 490.3125, 0.9375, 519.5, 322.96875, 0.92041015625, 440.0, 544.6875, 0.9189453125, 527.5, 516.5625, 0.9814453125, 484.75, 525.46875, 0.98193359375, 519.5, 583.125, 0.96826171875, 470.0, 606.09375, 0.96923828125, 524.5, 667.96875, 0.93603515625, 499.25, 676.875, 0.9365234375]]</t>
+          <t>[[0.0, 0.0, 244.59375, 262.546875, 63.84375, 231.5, 0.9214558601379395, 488.0, 378.28125, 0.98876953125, 497.75, 373.828125, 0.974609375, 481.0, 370.78125, 0.97607421875, 507.75, 384.375, 0.65234375, 467.25, 375.9375, 0.68798828125, 513.0, 409.453125, 0.97607421875, 452.75, 428.203125, 0.97900390625, 525.5, 370.78125, 0.93603515625, 451.5, 490.3125, 0.9375, 519.5, 322.96875, 0.92041015625, 440.0, 544.6875, 0.9189453125, 527.5, 516.5625, 0.9814453125, 484.75, 525.46875, 0.98193359375, 519.5, 583.125, 0.96826171875, 470.0, 606.09375, 0.96923828125, 524.5, 667.96875, 0.93603515625, 499.25, 676.875, 0.9365234375]]</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 258.2265625, 282.65625, 83.0625, 192.0, 0.9233980178833008, 504.75, 379.921875, 0.9814453125, 515.5, 376.875, 0.98095703125, 502.25, 373.125, 0.9365234375, 527.5, 389.296875, 0.8994140625, 489.0, 375.0, 0.705078125, 526.0, 418.125, 0.98388671875, 473.75, 429.609375, 0.982421875, 555.5, 416.953125, 0.95703125, 465.5, 487.03125, 0.95361328125, 572.0, 390.9375, 0.94775390625, 447.5, 525.0, 0.9423828125, 537.0, 530.15625, 0.98876953125, 494.75, 534.375, 0.98828125, 544.5, 605.15625, 0.978515625, 468.5, 609.84375, 0.9765625, 554.0, 671.71875, 0.943359375, 495.5, 677.8125, 0.94091796875]]</t>
+          <t>[[0.0, 0.0, 258.234375, 282.65625, 83.0625, 192.0, 0.9233980178833008, 504.75, 379.921875, 0.9814453125, 515.5, 376.875, 0.98095703125, 502.25, 373.125, 0.9365234375, 527.5, 389.296875, 0.8994140625, 489.0, 375.0, 0.705078125, 526.0, 418.125, 0.98388671875, 473.75, 429.609375, 0.982421875, 555.5, 416.953125, 0.95703125, 465.5, 487.03125, 0.95361328125, 572.0, 390.9375, 0.94775390625, 447.25, 525.0, 0.9423828125, 537.0, 530.15625, 0.98876953125, 494.75, 534.375, 0.98828125, 544.5, 605.15625, 0.97802734375, 468.5, 609.84375, 0.9765625, 554.0, 671.71875, 0.943359375, 495.5, 677.8125, 0.94091796875]]</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 264.921875, 287.21875, 90.625, 197.875, 0.9185748100280762, 522.0, 379.6875, 0.9931640625, 532.5, 377.8125, 0.98388671875, 518.0, 372.1875, 0.98291015625, 539.5, 389.0625, 0.75244140625, 503.75, 375.0, 0.74951171875, 540.0, 418.828125, 0.984375, 486.5, 421.171875, 0.98291015625, 573.5, 439.6875, 0.95263671875, 474.0, 465.234375, 0.9453125, 598.0, 429.609375, 0.9423828125, 456.0, 490.78125, 0.93505859375, 540.5, 533.4375, 0.984375, 497.0, 534.375, 0.9833984375, 554.0, 608.4375, 0.970703125, 470.25, 614.0625, 0.96875, 570.5, 692.8125, 0.93505859375, 495.5, 682.5, 0.93115234375]]</t>
+          <t>[[0.0, 0.0, 264.921875, 287.21875, 90.625, 197.875, 0.9185748100280762, 522.0, 379.6875, 0.9931640625, 532.5, 377.8125, 0.98388671875, 518.0, 372.1875, 0.98291015625, 539.5, 389.0625, 0.7529296875, 503.75, 375.0, 0.74951171875, 540.0, 418.828125, 0.984375, 486.5, 421.171875, 0.98291015625, 573.5, 439.6875, 0.95263671875, 474.0, 465.234375, 0.9453125, 598.0, 429.609375, 0.9423828125, 456.0, 490.78125, 0.93505859375, 540.5, 533.4375, 0.984375, 497.0, 534.375, 0.9833984375, 554.0, 608.4375, 0.970703125, 470.25, 614.0625, 0.96875, 570.5, 692.8125, 0.93505859375, 495.5, 682.5, 0.93115234375]]</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 272.375, 290.125, 92.4375, 203.25, 0.8926453590393066, 543.5, 379.21875, 0.9921875, 554.5, 377.34375, 0.98388671875, 539.0, 371.25, 0.97900390625, 562.0, 390.0, 0.7861328125, 525.0, 375.46875, 0.69921875, 557.5, 423.75, 0.98193359375, 506.75, 416.953125, 0.97998046875, 583.5, 460.78125, 0.94482421875, 485.25, 450.9375, 0.9345703125, 611.5, 475.78125, 0.93310546875, 462.5, 451.875, 0.921875, 547.0, 538.59375, 0.98193359375, 502.25, 536.25, 0.98095703125, 567.5, 617.34375, 0.96533203125, 475.0, 614.53125, 0.9619140625, 576.0, 706.875, 0.9248046875, 489.5, 683.4375, 0.919921875]]</t>
+          <t>[[0.0, 0.0, 272.375, 290.125, 92.4375, 203.25, 0.8926453590393066, 543.5, 379.21875, 0.9921875, 554.5, 377.34375, 0.98388671875, 539.0, 371.25, 0.97900390625, 562.0, 390.0, 0.7861328125, 525.0, 375.46875, 0.69970703125, 557.5, 423.75, 0.98193359375, 506.75, 416.953125, 0.97998046875, 583.5, 460.78125, 0.94482421875, 485.25, 450.9375, 0.9345703125, 611.5, 475.78125, 0.93310546875, 462.5, 451.875, 0.921875, 547.0, 538.59375, 0.98193359375, 502.25, 536.25, 0.98095703125, 567.5, 617.34375, 0.96533203125, 475.0, 614.53125, 0.9619140625, 576.0, 706.875, 0.9248046875, 489.5, 683.4375, 0.91943359375]]</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 271.109375, 292.28125, 81.375, 206.25, 0.9224162101745605, 569.5, 382.03125, 0.98974609375, 580.5, 379.6875, 0.9755859375, 566.0, 372.890625, 0.97509765625, 587.0, 393.515625, 0.7431640625, 551.0, 375.9375, 0.6875, 582.0, 431.25, 0.9736328125, 521.5, 411.09375, 0.97119140625, 600.0, 476.71875, 0.93408203125, 483.5, 418.125, 0.92041015625, 609.0, 513.75, 0.9228515625, 480.25, 398.90625, 0.90576171875, 553.0, 540.9375, 0.97900390625, 504.25, 534.84375, 0.9775390625, 578.0, 615.9375, 0.9580078125, 479.5, 614.0625, 0.953125, 578.0, 711.5625, 0.908203125, 485.0, 678.28125, 0.89990234375]]</t>
+          <t>[[0.0, 0.0, 271.109375, 292.28125, 81.375, 206.25, 0.9224162101745605, 569.5, 382.03125, 0.98974609375, 580.5, 379.6875, 0.9755859375, 566.0, 372.890625, 0.97509765625, 587.0, 393.515625, 0.74365234375, 551.0, 375.9375, 0.6875, 582.0, 431.25, 0.9736328125, 521.5, 411.09375, 0.97119140625, 600.0, 476.71875, 0.93408203125, 483.5, 418.125, 0.92041015625, 609.0, 513.75, 0.9228515625, 480.25, 398.90625, 0.90576171875, 553.0, 540.9375, 0.97900390625, 504.25, 534.84375, 0.9775390625, 578.0, 615.9375, 0.9580078125, 479.5, 614.0625, 0.953125, 578.0, 711.5625, 0.908203125, 485.0, 678.28125, 0.89990234375]]</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 272.3125, 290.65625, 80.1875, 211.75, 0.9238567352294922, 597.0, 388.125, 0.9921875, 607.5, 386.015625, 0.9775390625, 592.0, 379.453125, 0.98486328125, 612.5, 399.609375, 0.66357421875, 576.0, 384.609375, 0.748046875, 605.5, 447.890625, 0.978515625, 542.5, 408.75, 0.98046875, 606.5, 504.375, 0.93701171875, 498.75, 395.390625, 0.9443359375, 606.0, 549.84375, 0.9267578125, 494.75, 365.15625, 0.93115234375, 559.0, 544.21875, 0.9794921875, 507.75, 532.96875, 0.97998046875, 584.5, 619.21875, 0.958984375, 485.25, 615.9375, 0.9580078125, 579.5, 716.25, 0.9091796875, 485.75, 677.8125, 0.90771484375]]</t>
+          <t>[[0.0, 0.0, 272.3125, 290.65625, 80.1875, 211.75, 0.9243369102478027, 597.0, 388.125, 0.9921875, 607.5, 386.015625, 0.9775390625, 592.0, 379.453125, 0.98486328125, 612.5, 399.609375, 0.6640625, 576.0, 384.609375, 0.748046875, 605.5, 447.890625, 0.978515625, 542.5, 408.75, 0.98046875, 606.5, 504.375, 0.93701171875, 498.75, 395.625, 0.9443359375, 606.0, 549.84375, 0.9267578125, 494.75, 365.15625, 0.93115234375, 559.0, 544.21875, 0.9794921875, 507.75, 532.96875, 0.97998046875, 584.5, 619.21875, 0.958984375, 485.25, 615.9375, 0.9580078125, 580.0, 716.25, 0.9091796875, 485.75, 677.8125, 0.90771484375]]</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 278.84375, 279.3125, 92.875, 236.5, 0.9286584854125977, 626.0, 400.78125, 0.98876953125, 635.0, 398.4375, 0.92724609375, 620.5, 390.703125, 0.98681640625, 635.5, 408.75, 0.2374267578125, 601.5, 390.234375, 0.8427734375, 620.0, 459.609375, 0.9794921875, 559.5, 406.40625, 0.98291015625, 605.5, 521.71875, 0.93505859375, 516.5, 365.390625, 0.95703125, 602.0, 564.84375, 0.9248046875, 522.0, 316.640625, 0.94482421875, 563.5, 545.625, 0.98095703125, 511.5, 531.5625, 0.982421875, 587.5, 626.71875, 0.96435546875, 483.25, 629.0625, 0.9658203125, 579.0, 719.0625, 0.91845703125, 492.75, 667.03125, 0.91943359375]]</t>
+          <t>[[0.0, 0.0, 278.875, 279.3125, 92.875, 236.5, 0.9286584854125977, 626.0, 400.78125, 0.98876953125, 635.0, 398.4375, 0.92724609375, 620.5, 390.703125, 0.98681640625, 635.5, 408.75, 0.2381591796875, 601.5, 390.234375, 0.8427734375, 620.0, 459.609375, 0.9794921875, 559.5, 406.40625, 0.98291015625, 605.5, 521.71875, 0.93505859375, 516.5, 365.390625, 0.95703125, 602.0, 564.84375, 0.9248046875, 522.0, 316.640625, 0.94482421875, 563.5, 545.625, 0.98095703125, 511.5, 531.5625, 0.982421875, 587.5, 626.71875, 0.96435546875, 483.25, 629.0625, 0.9658203125, 579.0, 719.0625, 0.91845703125, 492.75, 667.03125, 0.91943359375]]</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 286.90625, 269.578125, 100.8125, 255.75, 0.92193603515625, 649.0, 418.359375, 0.97705078125, 657.0, 415.546875, 0.82275390625, 645.0, 408.28125, 0.97314453125, 655.0, 422.578125, 0.1322021484375, 623.0, 402.1875, 0.8837890625, 629.0, 468.515625, 0.978515625, 581.0, 408.28125, 0.98291015625, 602.0, 529.6875, 0.93212890625, 551.0, 349.6875, 0.96142578125, 601.0, 568.59375, 0.921875, 551.5, 295.3125, 0.94970703125, 566.5, 544.6875, 0.98046875, 517.0, 528.28125, 0.982421875, 586.5, 618.28125, 0.96630859375, 494.5, 625.78125, 0.96875, 579.5, 716.25, 0.9248046875, 490.25, 666.09375, 0.9267578125]]</t>
+          <t>[[0.0, 0.0, 286.90625, 269.578125, 100.8125, 255.75, 0.92193603515625, 649.0, 418.359375, 0.97705078125, 657.0, 415.546875, 0.822265625, 645.0, 408.28125, 0.97265625, 655.0, 422.578125, 0.1324462890625, 623.0, 402.1875, 0.8837890625, 629.0, 468.515625, 0.978515625, 581.0, 408.28125, 0.98291015625, 602.0, 529.6875, 0.93212890625, 551.0, 349.6875, 0.96142578125, 601.0, 568.59375, 0.921875, 551.5, 295.078125, 0.94970703125, 566.5, 544.6875, 0.98046875, 517.0, 528.28125, 0.982421875, 586.5, 618.28125, 0.96630859375, 494.5, 625.78125, 0.96875, 579.5, 716.25, 0.9248046875, 490.25, 666.09375, 0.9267578125]]</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 291.640625, 264.3125, 109.375, 265.25, 0.9286584854125977, 668.0, 435.234375, 0.97607421875, 675.0, 431.953125, 0.6591796875, 665.5, 424.921875, 0.9716796875, 671.5, 435.0, 0.04620361328125, 642.5, 414.140625, 0.8916015625, 630.0, 470.625, 0.97705078125, 604.0, 417.1875, 0.9794921875, 601.5, 526.40625, 0.93212890625, 600.0, 353.90625, 0.95947265625, 608.0, 566.71875, 0.91845703125, 610.5, 288.75, 0.9453125, 565.5, 544.6875, 0.97998046875, 524.5, 530.15625, 0.98095703125, 589.5, 619.21875, 0.9638671875, 518.0, 626.71875, 0.96484375, 579.0, 714.84375, 0.9140625, 492.75, 673.125, 0.912109375]]</t>
+          <t>[[0.0, 0.0, 291.640625, 264.3125, 109.375, 265.25, 0.9286584854125977, 668.0, 435.234375, 0.97607421875, 675.0, 431.953125, 0.6591796875, 665.5, 424.921875, 0.9716796875, 671.5, 435.0, 0.046112060546875, 642.5, 414.140625, 0.8916015625, 630.0, 470.625, 0.97705078125, 604.0, 417.1875, 0.9794921875, 601.5, 526.40625, 0.93212890625, 600.0, 353.90625, 0.95947265625, 608.0, 566.71875, 0.91845703125, 610.5, 288.75, 0.9453125, 565.5, 544.6875, 0.97998046875, 524.5, 530.15625, 0.98095703125, 590.0, 619.21875, 0.9638671875, 518.0, 626.71875, 0.96484375, 579.0, 714.84375, 0.9140625, 493.0, 673.125, 0.912109375]]</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 296.953125, 287.375, 112.875, 220.75, 0.9320197105407715, 679.0, 454.6875, 0.9794921875, 687.0, 448.59375, 0.65234375, 676.5, 443.90625, 0.986328125, 683.0, 441.09375, 0.0279541015625, 655.0, 429.140625, 0.89111328125, 637.0, 475.3125, 0.9716796875, 618.5, 434.0625, 0.974609375, 599.5, 522.1875, 0.91259765625, 646.5, 386.25, 0.951171875, 614.0, 562.96875, 0.8974609375, 676.0, 345.0, 0.931640625, 569.0, 542.34375, 0.97802734375, 529.5, 527.34375, 0.978515625, 593.0, 618.75, 0.9619140625, 537.0, 618.28125, 0.9638671875, 576.5, 713.4375, 0.91650390625, 498.5, 672.1875, 0.916015625]]</t>
+          <t>[[0.0, 0.0, 296.96875, 287.375, 112.875, 220.75, 0.9320197105407715, 679.0, 454.6875, 0.9794921875, 687.0, 448.59375, 0.65185546875, 676.5, 443.90625, 0.986328125, 683.0, 441.09375, 0.02801513671875, 655.0, 429.140625, 0.89111328125, 637.0, 475.3125, 0.9716796875, 618.5, 434.0625, 0.974609375, 599.5, 522.1875, 0.91259765625, 646.5, 386.25, 0.951171875, 614.0, 562.96875, 0.8974609375, 676.0, 345.0, 0.931640625, 569.0, 542.34375, 0.97802734375, 529.5, 527.34375, 0.978515625, 593.0, 618.75, 0.9619140625, 537.0, 618.28125, 0.9638671875, 576.5, 713.4375, 0.91650390625, 498.5, 672.1875, 0.916015625]]</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 314.171875, 305.9375, 139.625, 180.375, 0.9073770046234131, 693.5, 459.609375, 0.927734375, 700.5, 454.453125, 0.416259765625, 692.0, 449.53125, 0.9248046875, 693.0, 447.1875, 0.06842041015625, 669.0, 436.40625, 0.72216796875, 642.5, 472.96875, 0.953125, 629.5, 443.90625, 0.94677734375, 607.5, 520.78125, 0.9052734375, 678.0, 451.40625, 0.91259765625, 627.0, 562.5, 0.86767578125, 739.0, 453.28125, 0.88330078125, 566.5, 526.875, 0.96630859375, 532.5, 512.8125, 0.96337890625, 594.0, 615.46875, 0.9345703125, 552.0, 605.625, 0.9326171875, 573.0, 711.5625, 0.86376953125, 506.75, 681.5625, 0.8583984375]]</t>
+          <t>[[0.0, 0.0, 314.15625, 305.875, 139.5, 180.375, 0.9073770046234131, 693.5, 459.609375, 0.927734375, 700.5, 454.453125, 0.415771484375, 692.0, 449.53125, 0.92431640625, 692.5, 447.1875, 0.06842041015625, 669.0, 436.40625, 0.72216796875, 642.5, 472.96875, 0.953125, 629.5, 443.90625, 0.94677734375, 607.5, 520.78125, 0.9052734375, 678.0, 451.40625, 0.91259765625, 627.0, 562.5, 0.86767578125, 739.0, 453.28125, 0.88330078125, 566.5, 526.875, 0.96630859375, 532.5, 512.8125, 0.96337890625, 594.0, 615.46875, 0.9345703125, 552.0, 605.625, 0.9326171875, 573.0, 711.5625, 0.86376953125, 506.75, 681.5625, 0.8583984375]]</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 320.125, 307.34375, 134.375, 174.625, 0.9291386604309082, 702.5, 467.34375, 0.97265625, 710.0, 461.71875, 0.58544921875, 700.5, 457.5, 0.96337890625, 705.0, 451.875, 0.045684814453125, 680.0, 442.5, 0.91455078125, 655.5, 463.125, 0.97705078125, 646.0, 453.75, 0.9775390625, 608.5, 510.9375, 0.92724609375, 686.5, 510.9375, 0.95654296875, 628.5, 556.40625, 0.91162109375, 737.0, 554.0625, 0.9423828125, 579.0, 522.65625, 0.97705078125, 546.0, 511.40625, 0.97607421875, 604.0, 612.65625, 0.9609375, 570.0, 600.0, 0.96240234375, 577.0, 706.875, 0.912109375, 529.0, 686.25, 0.91015625]]</t>
+          <t>[[0.0, 0.0, 320.125, 307.34375, 134.375, 174.625, 0.9291386604309082, 702.5, 467.34375, 0.97265625, 710.0, 461.71875, 0.5859375, 700.5, 457.5, 0.96337890625, 705.0, 451.875, 0.0457763671875, 680.0, 442.5, 0.91455078125, 655.5, 463.125, 0.97705078125, 646.0, 453.75, 0.9775390625, 608.5, 510.9375, 0.92724609375, 686.5, 510.9375, 0.95654296875, 628.5, 556.40625, 0.91162109375, 737.0, 554.0625, 0.9423828125, 579.0, 522.65625, 0.97705078125, 546.0, 511.40625, 0.97607421875, 604.0, 612.65625, 0.9609375, 570.0, 600.0, 0.96240234375, 577.0, 706.875, 0.912109375, 529.0, 686.25, 0.91015625]]</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 315.15625, 308.0, 115.75, 172.875, 0.9329800605773926, 719.0, 471.09375, 0.94482421875, 725.0, 465.46875, 0.443115234375, 717.0, 460.78125, 0.95751953125, 716.5, 455.859375, 0.033782958984375, 696.0, 447.65625, 0.9169921875, 663.0, 462.65625, 0.96240234375, 661.0, 467.34375, 0.97705078125, 632.0, 519.84375, 0.8486328125, 681.0, 544.6875, 0.9521484375, 633.0, 545.15625, 0.826171875, 712.0, 607.96875, 0.92578125, 574.5, 516.09375, 0.9677734375, 555.0, 510.46875, 0.9736328125, 602.5, 608.4375, 0.953125, 587.5, 599.53125, 0.96484375, 564.0, 693.75, 0.9140625, 563.0, 698.4375, 0.92724609375]]</t>
+          <t>[[0.0, 0.0, 315.15625, 308.0, 115.75, 172.875, 0.9329800605773926, 719.0, 471.09375, 0.9443359375, 725.0, 465.46875, 0.442626953125, 717.0, 460.78125, 0.95751953125, 716.5, 455.859375, 0.033782958984375, 696.0, 447.65625, 0.9169921875, 663.0, 462.65625, 0.96240234375, 661.0, 467.34375, 0.97705078125, 632.0, 519.84375, 0.8486328125, 681.0, 545.15625, 0.9521484375, 633.0, 545.15625, 0.82666015625, 712.0, 607.5, 0.92578125, 574.5, 516.09375, 0.9677734375, 555.0, 510.46875, 0.9736328125, 602.5, 608.4375, 0.953125, 587.5, 599.53125, 0.96484375, 564.0, 693.75, 0.9140625, 563.0, 698.4375, 0.92724609375]]</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 322.09375, 308.34375, 120.125, 167.375, 0.9397025108337402, 737.0, 477.1875, 0.97021484375, 743.5, 471.09375, 0.55126953125, 735.0, 466.875, 0.9794921875, 734.5, 462.421875, 0.03424072265625, 711.0, 453.75, 0.92822265625, 677.5, 465.0, 0.92236328125, 678.5, 475.078125, 0.97607421875, 648.0, 537.1875, 0.560546875, 669.5, 555.0, 0.9462890625, 653.5, 591.5625, 0.51708984375, 676.5, 616.40625, 0.90087890625, 574.5, 512.8125, 0.94091796875, 565.0, 511.40625, 0.966796875, 607.5, 602.8125, 0.92822265625, 599.5, 604.6875, 0.96435546875, 574.0, 690.9375, 0.90478515625, 593.0, 706.40625, 0.939453125]]</t>
+          <t>[[0.0, 0.0, 322.09375, 308.34375, 120.125, 167.375, 0.9397025108337402, 737.0, 477.1875, 0.97021484375, 743.5, 471.09375, 0.55078125, 735.0, 466.875, 0.9794921875, 734.5, 462.421875, 0.034088134765625, 711.0, 453.75, 0.92822265625, 677.5, 465.0, 0.92236328125, 678.5, 475.3125, 0.97607421875, 648.0, 537.1875, 0.560546875, 669.5, 555.0, 0.9462890625, 653.5, 591.5625, 0.51708984375, 676.5, 616.40625, 0.90087890625, 574.5, 512.8125, 0.94091796875, 565.0, 511.40625, 0.966796875, 607.5, 602.8125, 0.92822265625, 599.5, 604.6875, 0.96435546875, 574.0, 690.9375, 0.90478515625, 593.0, 706.40625, 0.939453125]]</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 334.609375, 317.03125, 125.125, 175.75, 0.9358611106872559, 773.0, 491.71875, 0.96728515625, 780.0, 482.34375, 0.307373046875, 770.5, 480.9375, 0.97705078125, 753.0, 464.0625, 0.019561767578125, 744.5, 469.21875, 0.89501953125, 702.0, 452.578125, 0.92626953125, 706.5, 495.0, 0.94921875, 641.0, 442.03125, 0.6162109375, 644.0, 538.59375, 0.81494140625, 649.5, 466.640625, 0.50439453125, 639.0, 521.71875, 0.70556640625, 584.0, 515.625, 0.9501953125, 591.0, 528.28125, 0.955078125, 607.5, 615.9375, 0.94482421875, 632.5, 627.65625, 0.95458984375, 573.5, 707.8125, 0.927734375, 658.5, 731.71875, 0.93408203125]]</t>
+          <t>[[0.0, 0.0, 334.609375, 317.03125, 125.125, 175.75, 0.9358611106872559, 773.0, 491.71875, 0.96728515625, 780.0, 482.34375, 0.307861328125, 770.5, 480.9375, 0.97705078125, 753.0, 464.0625, 0.019561767578125, 744.5, 469.21875, 0.89501953125, 702.0, 452.578125, 0.92626953125, 706.5, 495.0, 0.94921875, 641.0, 442.03125, 0.61572265625, 644.0, 538.59375, 0.814453125, 649.5, 466.640625, 0.50390625, 639.0, 521.71875, 0.70458984375, 584.0, 515.625, 0.9501953125, 591.0, 528.28125, 0.95458984375, 607.5, 615.9375, 0.94482421875, 632.5, 627.65625, 0.95458984375, 573.5, 707.8125, 0.927734375, 658.0, 731.71875, 0.93408203125]]</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 339.28125, 318.2890625, 132.625, 187.0, 0.9387421607971191, 787.5, 493.59375, 0.95556640625, 794.5, 484.6875, 0.267333984375, 786.0, 482.8125, 0.9609375, 773.0, 466.171875, 0.01512908935546875, 763.0, 469.21875, 0.8330078125, 719.0, 453.984375, 0.94677734375, 724.5, 488.4375, 0.9287109375, 653.5, 432.65625, 0.869140625, 675.5, 503.4375, 0.7705078125, 632.0, 452.8125, 0.81982421875, 634.5, 474.609375, 0.70556640625, 604.0, 521.71875, 0.97216796875, 611.5, 529.6875, 0.96337890625, 620.0, 622.96875, 0.96728515625, 653.0, 632.8125, 0.9580078125, 575.0, 706.875, 0.9423828125, 670.5, 742.96875, 0.9287109375]]</t>
+          <t>[[0.0, 0.0, 339.28125, 318.2890625, 132.625, 187.0, 0.9387421607971191, 787.5, 493.125, 0.95556640625, 794.5, 484.6875, 0.267333984375, 786.0, 482.8125, 0.9609375, 773.0, 466.171875, 0.01512908935546875, 763.0, 469.21875, 0.8330078125, 719.0, 453.984375, 0.94677734375, 724.5, 488.4375, 0.9287109375, 653.5, 432.65625, 0.869140625, 675.5, 503.4375, 0.77099609375, 632.0, 452.8125, 0.81982421875, 634.5, 474.609375, 0.70556640625, 604.0, 521.71875, 0.97216796875, 611.5, 529.6875, 0.96337890625, 620.0, 622.96875, 0.96728515625, 653.0, 632.8125, 0.9580078125, 575.0, 706.875, 0.9423828125, 670.5, 742.96875, 0.9287109375]]</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 345.65625, 316.578125, 137.625, 194.25, 0.9392359256744385, 804.0, 488.4375, 0.91015625, 811.0, 478.125, 0.147705078125, 804.0, 476.25, 0.931640625, 777.0, 463.125, 0.0251312255859375, 778.0, 467.34375, 0.86962890625, 728.5, 450.46875, 0.9365234375, 746.0, 486.09375, 0.95458984375, 680.5, 427.96875, 0.76806640625, 694.0, 479.0625, 0.88623046875, 640.0, 416.015625, 0.74365234375, 646.0, 460.3125, 0.84814453125, 619.0, 519.375, 0.978515625, 636.5, 532.5, 0.97998046875, 634.5, 617.8125, 0.978515625, 681.0, 634.6875, 0.982421875, 578.0, 697.96875, 0.95849609375, 680.0, 745.3125, 0.96337890625]]</t>
+          <t>[[0.0, 0.0, 345.65625, 316.578125, 137.625, 194.25, 0.9392359256744385, 804.0, 488.4375, 0.91015625, 811.0, 478.125, 0.147705078125, 804.0, 476.25, 0.931640625, 777.0, 463.125, 0.0251312255859375, 778.0, 467.34375, 0.86962890625, 728.5, 450.46875, 0.9365234375, 746.0, 486.09375, 0.95458984375, 680.5, 427.96875, 0.76806640625, 693.5, 479.0625, 0.88623046875, 640.0, 416.25, 0.74365234375, 646.0, 460.3125, 0.84814453125, 619.0, 519.375, 0.978515625, 636.5, 532.5, 0.97998046875, 634.5, 617.8125, 0.978515625, 681.0, 634.6875, 0.982421875, 578.0, 697.96875, 0.95849609375, 680.0, 745.3125, 0.96337890625]]</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 351.5234375, 312.65625, 139.0, 203.25, 0.9411430358886719, 821.5, 475.78125, 0.95947265625, 828.5, 465.46875, 0.254150390625, 817.5, 464.765625, 0.9658203125, 800.0, 446.25, 0.0261993408203125, 792.0, 454.6875, 0.89697265625, 747.0, 442.03125, 0.96826171875, 763.5, 494.53125, 0.9560546875, 694.0, 423.28125, 0.89697265625, 708.5, 543.28125, 0.7919921875, 646.5, 406.875, 0.84521484375, 669.0, 536.71875, 0.71533203125, 634.0, 526.875, 0.97314453125, 655.0, 542.8125, 0.9638671875, 650.5, 628.125, 0.96240234375, 694.0, 639.375, 0.95068359375, 588.5, 694.21875, 0.92431640625, 673.0, 749.0625, 0.90576171875]]</t>
+          <t>[[0.0, 0.0, 351.5390625, 312.65625, 139.0, 203.25, 0.9406628608703613, 821.5, 475.78125, 0.95947265625, 828.5, 465.46875, 0.253662109375, 817.5, 464.765625, 0.9658203125, 800.0, 446.25, 0.0261993408203125, 792.0, 454.6875, 0.89697265625, 746.5, 442.03125, 0.96826171875, 763.5, 494.53125, 0.9560546875, 694.0, 423.28125, 0.89697265625, 708.5, 543.28125, 0.7919921875, 646.5, 406.875, 0.84521484375, 669.0, 536.71875, 0.71484375, 634.0, 526.875, 0.97314453125, 655.0, 543.28125, 0.9638671875, 650.5, 628.125, 0.96240234375, 694.0, 639.375, 0.95068359375, 588.5, 694.21875, 0.92431640625, 673.0, 749.0625, 0.90576171875]]</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 357.9375, 309.890625, 142.125, 211.125, 0.9401099681854248, 840.0, 460.3125, 0.966796875, 844.0, 451.171875, 0.43017578125, 834.5, 450.0, 0.9775390625, 816.0, 435.46875, 0.038177490234375, 808.0, 440.625, 0.73291015625, 757.0, 430.546875, 0.93310546875, 782.0, 481.40625, 0.9404296875, 697.5, 413.90625, 0.869140625, 740.0, 537.1875, 0.88134765625, 655.5, 401.25, 0.81689453125, 747.0, 508.125, 0.82568359375, 648.5, 525.9375, 0.9609375, 672.0, 541.40625, 0.9609375, 669.0, 628.125, 0.9345703125, 701.0, 645.9375, 0.9365234375, 598.0, 685.78125, 0.87841796875, 671.0, 749.0625, 0.8779296875]]</t>
+          <t>[[0.0, 0.0, 357.9375, 309.90625, 142.125, 211.125, 0.9401099681854248, 839.5, 460.3125, 0.966796875, 844.0, 451.171875, 0.4306640625, 834.5, 450.0, 0.9775390625, 815.5, 435.46875, 0.038238525390625, 808.0, 440.625, 0.7333984375, 757.0, 430.546875, 0.93310546875, 782.0, 481.40625, 0.9404296875, 697.5, 413.90625, 0.869140625, 740.0, 537.1875, 0.88134765625, 655.5, 401.25, 0.81689453125, 747.0, 508.125, 0.82568359375, 648.5, 525.9375, 0.9609375, 672.0, 541.40625, 0.9609375, 669.0, 628.125, 0.9345703125, 701.0, 645.9375, 0.9365234375, 598.0, 685.78125, 0.87841796875, 671.0, 749.53125, 0.8779296875]]</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 365.359375, 308.75, 141.625, 211.75, 0.9416232109069824, 857.0, 445.78125, 0.9599609375, 862.0, 436.40625, 0.294189453125, 853.0, 435.46875, 0.97021484375, 836.0, 424.453125, 0.02752685546875, 825.5, 427.03125, 0.92236328125, 774.0, 423.75, 0.96923828125, 801.0, 469.453125, 0.97607421875, 712.0, 405.9375, 0.90869140625, 763.5, 523.125, 0.94580078125, 659.5, 394.21875, 0.8876953125, 755.5, 546.5625, 0.92529296875, 673.5, 525.0, 0.97998046875, 689.5, 537.65625, 0.98046875, 693.5, 625.3125, 0.97021484375, 710.5, 642.1875, 0.97314453125, 618.5, 686.25, 0.93798828125, 671.0, 745.78125, 0.93896484375]]</t>
+          <t>[[0.0, 0.0, 365.375, 308.75, 141.625, 211.75, 0.9416232109069824, 857.0, 445.78125, 0.9599609375, 862.0, 436.40625, 0.294189453125, 853.0, 435.46875, 0.97021484375, 836.0, 424.453125, 0.027435302734375, 825.5, 427.03125, 0.92236328125, 774.0, 423.75, 0.96923828125, 801.0, 469.453125, 0.97607421875, 712.0, 405.9375, 0.90869140625, 763.5, 523.125, 0.94580078125, 659.5, 394.21875, 0.88720703125, 755.5, 546.5625, 0.92529296875, 673.5, 525.0, 0.97998046875, 689.5, 537.65625, 0.98046875, 693.5, 625.3125, 0.97021484375, 710.5, 642.1875, 0.97314453125, 618.5, 686.25, 0.93798828125, 671.0, 745.78125, 0.93896484375]]</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 375.53125, 305.8125, 145.25, 217.125, 0.9434795379638672, 877.0, 429.84375, 0.9677734375, 881.0, 420.703125, 0.248291015625, 873.0, 418.828125, 0.9833984375, 844.0, 409.921875, 0.0190582275390625, 845.5, 412.03125, 0.77880859375, 792.5, 411.5625, 0.9560546875, 821.0, 456.09375, 0.95947265625, 722.0, 403.125, 0.90625, 782.0, 520.78125, 0.92333984375, 665.0, 399.84375, 0.86181640625, 787.5, 552.65625, 0.88720703125, 689.5, 515.15625, 0.9677734375, 708.0, 529.21875, 0.96728515625, 701.0, 621.09375, 0.9306640625, 714.0, 639.375, 0.93212890625, 637.0, 687.1875, 0.84814453125, 671.0, 744.375, 0.84521484375]]</t>
+          <t>[[0.0, 0.0, 375.53125, 305.8125, 145.25, 217.125, 0.9434795379638672, 877.0, 429.84375, 0.9677734375, 881.0, 420.703125, 0.248291015625, 873.0, 418.828125, 0.9833984375, 844.0, 409.921875, 0.0190582275390625, 845.5, 412.03125, 0.77880859375, 792.5, 411.5625, 0.9560546875, 821.0, 456.328125, 0.95947265625, 722.0, 403.125, 0.90625, 782.0, 520.78125, 0.92333984375, 665.0, 399.84375, 0.861328125, 787.5, 553.125, 0.88720703125, 689.5, 515.15625, 0.9677734375, 707.5, 529.21875, 0.96728515625, 701.0, 621.09375, 0.9306640625, 714.0, 639.375, 0.93212890625, 637.0, 687.1875, 0.84814453125, 671.0, 744.375, 0.84521484375]]</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 384.109375, 302.5, 146.0, 224.25, 0.9349007606506348, 898.5, 417.1875, 0.97607421875, 903.0, 407.8125, 0.387451171875, 893.5, 406.40625, 0.98486328125, 877.0, 399.375, 0.0225372314453125, 863.5, 396.796875, 0.9375, 812.5, 406.875, 0.97265625, 838.5, 438.28125, 0.98095703125, 737.0, 407.34375, 0.91796875, 803.0, 508.125, 0.96435546875, 675.0, 412.734375, 0.900390625, 815.5, 554.0625, 0.951171875, 726.0, 515.15625, 0.984375, 726.0, 522.65625, 0.98583984375, 741.0, 618.75, 0.97900390625, 711.5, 634.21875, 0.982421875, 655.0, 685.3125, 0.95703125, 677.5, 742.03125, 0.95947265625]]</t>
+          <t>[[0.0, 0.0, 384.109375, 302.5, 146.0, 224.25, 0.9349007606506348, 898.5, 417.1875, 0.97607421875, 903.0, 407.8125, 0.38671875, 893.5, 406.40625, 0.984375, 877.0, 399.375, 0.0225372314453125, 863.5, 396.796875, 0.9375, 812.5, 406.875, 0.97216796875, 838.5, 438.28125, 0.98095703125, 737.0, 407.34375, 0.91796875, 803.0, 508.125, 0.96435546875, 675.5, 412.96875, 0.900390625, 815.5, 553.59375, 0.951171875, 726.0, 515.15625, 0.984375, 726.0, 522.65625, 0.98583984375, 741.0, 618.75, 0.97900390625, 711.5, 634.6875, 0.982421875, 655.0, 685.3125, 0.95703125, 677.5, 742.03125, 0.95947265625]]</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 393.828125, 299.546875, 147.5, 232.125, 0.9353809356689453, 919.5, 402.421875, 0.978515625, 923.5, 393.75, 0.47314453125, 914.0, 391.40625, 0.98681640625, 902.0, 388.359375, 0.0230255126953125, 883.5, 382.03125, 0.935546875, 834.0, 401.25, 0.97119140625, 860.5, 422.109375, 0.9794921875, 749.5, 408.75, 0.919921875, 825.5, 492.65625, 0.96044921875, 685.0, 425.15625, 0.90380859375, 835.0, 543.28125, 0.94677734375, 755.0, 515.625, 0.98291015625, 741.0, 516.09375, 0.984375, 764.0, 618.75, 0.97412109375, 715.5, 623.4375, 0.9765625, 706.0, 708.28125, 0.94287109375, 670.0, 724.21875, 0.94384765625]]</t>
+          <t>[[0.0, 0.0, 393.0, 299.75, 148.5, 231.375, 0.9357776641845703, 915.5, 402.1875, 0.970703125, 920.5, 393.984375, 0.376953125, 910.0, 390.46875, 0.984375, 892.5, 386.71875, 0.023193359375, 882.0, 382.03125, 0.75634765625, 828.0, 398.4375, 0.94482421875, 860.0, 423.75, 0.96337890625, 750.0, 402.890625, 0.89453125, 824.5, 493.59375, 0.93212890625, 689.5, 421.171875, 0.85693359375, 837.0, 541.875, 0.890625, 749.0, 512.34375, 0.96923828125, 744.5, 514.6875, 0.97314453125, 760.0, 620.625, 0.931640625, 719.5, 622.96875, 0.939453125, 704.5, 712.5, 0.8447265625, 673.5, 727.5, 0.85302734375]]</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 397.6875, 294.5, 157.75, 237.25, 0.932889461517334, 936.0, 389.0625, 0.9853515625, 940.0, 380.390625, 0.46484375, 929.5, 377.578125, 0.99072265625, 916.5, 375.46875, 0.019195556640625, 901.5, 370.3125, 0.7685546875, 857.0, 393.515625, 0.95458984375, 878.5, 408.75, 0.9638671875, 773.0, 410.15625, 0.90771484375, 841.0, 481.40625, 0.93310546875, 711.5, 438.75, 0.86767578125, 853.0, 534.84375, 0.89697265625, 777.0, 511.875, 0.97314453125, 760.5, 508.59375, 0.974609375, 791.0, 620.625, 0.94140625, 725.0, 617.34375, 0.94384765625, 748.0, 724.21875, 0.86474609375, 667.5, 717.1875, 0.865234375]]</t>
+          <t>[[0.0, 0.0, 397.6875, 294.5, 157.75, 237.25, 0.932889461517334, 936.0, 389.0625, 0.9853515625, 940.0, 380.390625, 0.465087890625, 929.5, 377.578125, 0.99072265625, 916.5, 375.46875, 0.019195556640625, 901.5, 370.3125, 0.7685546875, 857.0, 393.515625, 0.95458984375, 878.5, 408.75, 0.9638671875, 773.0, 410.15625, 0.90771484375, 841.0, 481.40625, 0.93310546875, 711.5, 438.75, 0.86767578125, 853.0, 534.375, 0.89697265625, 777.0, 511.875, 0.97314453125, 760.5, 508.59375, 0.974609375, 791.0, 620.625, 0.94140625, 725.0, 617.34375, 0.94384765625, 748.0, 724.21875, 0.86474609375, 667.5, 717.1875, 0.865234375]]</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 400.09375, 289.25, 172.25, 238.75, 0.9357776641845703, 956.0, 378.75, 0.9833984375, 959.5, 369.84375, 0.4306640625, 949.0, 366.796875, 0.9892578125, 933.5, 367.5, 0.0179901123046875, 917.5, 360.9375, 0.76318359375, 876.0, 390.9375, 0.95458984375, 896.5, 396.09375, 0.96484375, 793.0, 424.21875, 0.91259765625, 864.5, 465.46875, 0.93603515625, 738.0, 463.828125, 0.8779296875, 874.0, 518.90625, 0.9013671875, 802.5, 511.875, 0.9736328125, 782.0, 505.3125, 0.9755859375, 818.0, 621.5625, 0.94287109375, 735.0, 611.25, 0.9453125, 800.0, 736.875, 0.86572265625, 657.5, 699.84375, 0.8671875]]</t>
+          <t>[[0.0, 0.0, 400.09375, 289.25, 172.25, 238.75, 0.9357776641845703, 956.0, 378.75, 0.9833984375, 959.5, 369.84375, 0.43017578125, 949.0, 366.796875, 0.98974609375, 933.5, 367.5, 0.017913818359375, 917.5, 360.9375, 0.76318359375, 876.0, 390.9375, 0.95458984375, 896.5, 396.09375, 0.96484375, 793.0, 424.21875, 0.91259765625, 864.5, 465.46875, 0.93603515625, 738.0, 463.828125, 0.8779296875, 874.0, 518.90625, 0.9013671875, 802.5, 512.34375, 0.9736328125, 782.0, 505.3125, 0.9755859375, 818.0, 621.5625, 0.94287109375, 735.0, 611.25, 0.9453125, 800.0, 736.875, 0.8662109375, 657.5, 699.84375, 0.8671875]]</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 402.5, 290.15625, 185.0, 245.625, 0.9397025108337402, 976.5, 374.53125, 0.970703125, 979.5, 365.390625, 0.406005859375, 971.0, 361.40625, 0.9736328125, 948.5, 362.8125, 0.0301513671875, 936.0, 354.140625, 0.9384765625, 902.0, 390.46875, 0.89013671875, 913.0, 388.828125, 0.982421875, 836.5, 455.625, 0.4599609375, 882.5, 461.953125, 0.96533203125, 804.5, 507.65625, 0.4541015625, 889.0, 522.65625, 0.92919921875, 826.5, 512.34375, 0.951171875, 801.0, 504.84375, 0.98095703125, 846.0, 625.3125, 0.943359375, 744.0, 611.71875, 0.97802734375, 851.0, 746.25, 0.9169921875, 650.0, 683.90625, 0.95703125]]</t>
+          <t>[[0.0, 0.0, 402.5, 290.125, 185.0, 245.625, 0.9397025108337402, 977.0, 374.53125, 0.970703125, 979.5, 365.390625, 0.4052734375, 971.0, 361.40625, 0.9736328125, 948.5, 362.8125, 0.0301513671875, 936.0, 354.140625, 0.9384765625, 902.0, 390.46875, 0.89013671875, 913.0, 388.828125, 0.982421875, 836.5, 455.625, 0.459228515625, 882.5, 461.953125, 0.96533203125, 805.0, 507.65625, 0.45361328125, 889.0, 522.65625, 0.92919921875, 826.5, 512.34375, 0.951171875, 801.0, 504.84375, 0.98095703125, 846.0, 625.3125, 0.943359375, 744.0, 611.71875, 0.97802734375, 851.0, 746.25, 0.91650390625, 650.0, 683.90625, 0.95703125]]</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 405.1875, 293.046875, 198.75, 252.5, 0.9416232109069824, 992.0, 372.1875, 0.92919921875, 995.5, 364.21875, 0.31005859375, 987.0, 359.296875, 0.94775390625, 970.0, 365.15625, 0.03033447265625, 952.5, 352.03125, 0.9296875, 924.0, 392.34375, 0.84619140625, 932.0, 390.703125, 0.978515625, 878.5, 464.0625, 0.390625, 902.0, 465.9375, 0.9658203125, 890.0, 525.46875, 0.4169921875, 913.0, 530.625, 0.9326171875, 857.0, 524.0625, 0.9443359375, 830.5, 514.6875, 0.98046875, 877.5, 632.8125, 0.94189453125, 765.0, 616.40625, 0.97998046875, 889.0, 751.40625, 0.92138671875, 649.0, 663.75, 0.96337890625]]</t>
+          <t>[[0.0, 0.0, 405.21875, 293.03125, 198.75, 252.5, 0.9416232109069824, 992.5, 372.1875, 0.92919921875, 995.5, 363.984375, 0.309326171875, 987.0, 359.0625, 0.9482421875, 970.0, 365.15625, 0.03021240234375, 952.5, 352.03125, 0.9296875, 924.0, 392.34375, 0.84619140625, 932.0, 390.703125, 0.978515625, 878.5, 464.0625, 0.390380859375, 902.0, 465.9375, 0.9658203125, 890.0, 525.46875, 0.416748046875, 913.0, 530.625, 0.9326171875, 857.0, 524.0625, 0.9443359375, 830.5, 514.6875, 0.98046875, 877.5, 632.8125, 0.94189453125, 765.0, 616.40625, 0.97998046875, 889.0, 751.40625, 0.92138671875, 649.0, 663.75, 0.96337890625]]</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 409.03125, 297.1875, 205.5, 257.75, 0.9434795379638672, 1007.0, 372.65625, 0.9619140625, 1010.0, 364.21875, 0.2384033203125, 1000.0, 360.9375, 0.9794921875, 984.0, 365.625, 0.010528564453125, 968.0, 357.890625, 0.7783203125, 943.0, 400.078125, 0.83984375, 948.0, 397.265625, 0.9580078125, 900.5, 472.734375, 0.544921875, 914.5, 469.6875, 0.927734375, 907.5, 536.25, 0.496337890625, 928.0, 538.125, 0.87060546875, 879.0, 534.375, 0.92138671875, 849.0, 524.0625, 0.95849609375, 911.0, 642.1875, 0.8974609375, 778.5, 624.375, 0.9404296875, 919.5, 767.8125, 0.83984375, 659.0, 640.78125, 0.8828125]]</t>
+          <t>[[0.0, 0.0, 409.03125, 297.1875, 205.5, 257.75, 0.9434795379638672, 1007.0, 372.65625, 0.9619140625, 1009.5, 364.21875, 0.2381591796875, 1000.0, 360.703125, 0.9794921875, 984.0, 365.625, 0.010528564453125, 968.0, 357.890625, 0.77783203125, 943.0, 400.078125, 0.83984375, 948.0, 397.265625, 0.9580078125, 900.5, 472.734375, 0.544921875, 914.5, 469.6875, 0.927734375, 907.5, 536.25, 0.496337890625, 928.0, 538.125, 0.87060546875, 879.0, 534.375, 0.92138671875, 849.0, 524.0625, 0.95849609375, 911.0, 642.1875, 0.89794921875, 778.5, 624.375, 0.9404296875, 919.5, 767.8125, 0.84033203125, 659.0, 640.78125, 0.8828125]]</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 416.8125, 301.75, 204.625, 261.5, 0.9430637359619141, 1027.0, 377.34375, 0.9521484375, 1030.0, 367.96875, 0.398681640625, 1019.0, 365.15625, 0.9599609375, 1011.0, 370.078125, 0.034027099609375, 984.5, 363.515625, 0.94580078125, 968.5, 406.40625, 0.8603515625, 960.0, 404.53125, 0.982421875, 920.0, 474.375, 0.38916015625, 928.5, 477.1875, 0.97021484375, 925.0, 543.28125, 0.4140625, 943.0, 549.84375, 0.939453125, 916.0, 546.5625, 0.9462890625, 872.5, 537.1875, 0.9814453125, 944.0, 652.5, 0.9404296875, 797.5, 642.65625, 0.9794921875, 926.5, 778.59375, 0.921875, 679.5, 637.03125, 0.96337890625]]</t>
+          <t>[[0.0, 0.0, 416.8125, 301.75, 204.625, 261.5, 0.9430637359619141, 1027.0, 377.34375, 0.9521484375, 1030.0, 367.96875, 0.39794921875, 1019.0, 365.15625, 0.9599609375, 1011.0, 370.3125, 0.034027099609375, 984.5, 363.515625, 0.94580078125, 968.5, 406.40625, 0.8603515625, 960.0, 404.53125, 0.982421875, 920.0, 474.375, 0.38916015625, 928.5, 477.1875, 0.97021484375, 925.0, 543.28125, 0.413818359375, 943.0, 549.84375, 0.939453125, 916.0, 546.5625, 0.9462890625, 872.5, 537.1875, 0.9814453125, 944.0, 652.5, 0.9404296875, 797.5, 642.65625, 0.9794921875, 926.5, 778.59375, 0.921875, 679.5, 637.03125, 0.962890625]]</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 430.5625, 302.140625, 195.125, 260.25, 0.9411430358886719, 1045.0, 376.875, 0.95556640625, 1048.0, 367.96875, 0.45703125, 1036.0, 364.6875, 0.95947265625, 1027.0, 372.1875, 0.038970947265625, 1001.5, 365.15625, 0.94189453125, 987.5, 411.796875, 0.859375, 975.5, 409.21875, 0.98291015625, 939.5, 485.15625, 0.382568359375, 938.0, 483.75, 0.97119140625, 950.0, 558.28125, 0.405029296875, 960.5, 559.6875, 0.94140625, 934.5, 555.9375, 0.94482421875, 895.0, 548.4375, 0.9814453125, 968.0, 654.375, 0.9404296875, 835.5, 657.1875, 0.98046875, 928.5, 780.9375, 0.92529296875, 715.0, 636.5625, 0.96630859375]]</t>
+          <t>[[0.0, 0.0, 430.5625, 302.125, 195.125, 260.25, 0.9411430358886719, 1045.0, 376.875, 0.95556640625, 1048.0, 367.96875, 0.45751953125, 1036.0, 364.6875, 0.9599609375, 1027.0, 372.1875, 0.038970947265625, 1001.5, 365.15625, 0.94189453125, 987.5, 411.5625, 0.859375, 975.5, 409.21875, 0.98291015625, 939.5, 485.15625, 0.382568359375, 938.0, 483.75, 0.97119140625, 950.0, 558.28125, 0.405029296875, 960.5, 559.6875, 0.94140625, 934.5, 555.9375, 0.94482421875, 895.0, 548.4375, 0.9814453125, 968.0, 654.375, 0.9404296875, 835.5, 657.1875, 0.98046875, 928.0, 780.9375, 0.92529296875, 715.0, 636.5625, 0.96630859375]]</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 446.2421875, 301.6875, 184.75, 261.75, 0.9397025108337402, 1064.0, 374.0625, 0.96484375, 1068.0, 365.390625, 0.387451171875, 1056.0, 362.34375, 0.974609375, 1052.0, 369.375, 0.0190887451171875, 1020.5, 363.046875, 0.95068359375, 1014.0, 415.3125, 0.9541015625, 990.0, 405.0, 0.984375, 979.0, 501.5625, 0.7890625, 946.0, 475.78125, 0.97119140625, 998.5, 576.09375, 0.78515625, 971.5, 556.875, 0.955078125, 960.0, 555.46875, 0.97412109375, 919.5, 547.03125, 0.984375, 981.5, 661.875, 0.962890625, 878.5, 666.5625, 0.9775390625, 927.5, 780.0, 0.93115234375, 760.0, 645.9375, 0.95068359375]]</t>
+          <t>[[0.0, 0.0, 446.234375, 301.6875, 184.75, 261.75, 0.9397025108337402, 1064.0, 374.0625, 0.96484375, 1068.0, 365.390625, 0.387451171875, 1056.0, 362.34375, 0.974609375, 1052.0, 369.375, 0.0190887451171875, 1021.0, 363.046875, 0.95068359375, 1014.0, 415.078125, 0.9541015625, 990.0, 405.0, 0.984375, 979.0, 501.5625, 0.78955078125, 946.0, 475.78125, 0.97119140625, 998.5, 576.09375, 0.78564453125, 971.5, 556.875, 0.955078125, 960.0, 555.46875, 0.97412109375, 919.5, 547.03125, 0.984375, 981.5, 661.875, 0.962890625, 878.5, 666.5625, 0.9775390625, 927.5, 780.0, 0.93115234375, 760.0, 645.9375, 0.95068359375]]</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 465.8125, 298.6875, 165.75, 265.5, 0.9401826858520508, 1085.0, 365.390625, 0.955078125, 1088.0, 356.25, 0.459228515625, 1077.0, 353.90625, 0.96728515625, 1072.0, 358.59375, 0.027801513671875, 1041.0, 352.96875, 0.93603515625, 1042.0, 411.328125, 0.97216796875, 1010.0, 395.625, 0.98486328125, 1010.0, 498.75, 0.9169921875, 955.0, 460.3125, 0.9716796875, 1046.0, 565.3125, 0.9140625, 976.0, 534.84375, 0.9619140625, 984.0, 552.65625, 0.98388671875, 945.0, 543.75, 0.9873046875, 991.0, 666.5625, 0.97412109375, 930.5, 671.25, 0.9794921875, 928.5, 780.0, 0.9375, 808.5, 656.25, 0.94677734375]]</t>
+          <t>[[0.0, 0.0, 465.8125, 298.6875, 165.75, 265.5, 0.9397025108337402, 1085.0, 365.15625, 0.955078125, 1088.0, 356.015625, 0.459228515625, 1077.0, 353.90625, 0.966796875, 1072.0, 358.59375, 0.0278472900390625, 1041.0, 352.96875, 0.93603515625, 1042.0, 411.328125, 0.97216796875, 1010.0, 395.625, 0.98486328125, 1010.0, 498.75, 0.9169921875, 955.0, 460.3125, 0.9716796875, 1046.0, 565.3125, 0.9140625, 976.0, 534.84375, 0.9619140625, 984.0, 552.65625, 0.9833984375, 945.0, 543.75, 0.9873046875, 991.0, 666.5625, 0.97412109375, 930.5, 671.25, 0.9794921875, 928.5, 780.0, 0.9375, 808.5, 656.25, 0.94677734375]]</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 489.125, 295.25, 158.375, 271.5, 0.9411430358886719, 1107.0, 352.96875, 0.97021484375, 1110.0, 344.296875, 0.47802734375, 1099.0, 341.25, 0.97705078125, 1091.0, 348.515625, 0.0280609130859375, 1063.0, 340.3125, 0.947265625, 1062.0, 404.53125, 0.97802734375, 1031.0, 382.265625, 0.98486328125, 1037.0, 496.40625, 0.93115234375, 964.0, 438.984375, 0.9716796875, 1086.0, 546.5625, 0.927734375, 994.0, 521.25, 0.96435546875, 1009.5, 546.09375, 0.98583984375, 974.5, 535.3125, 0.98779296875, 1002.0, 669.375, 0.9755859375, 979.0, 664.21875, 0.97900390625, 932.0, 779.0625, 0.9306640625, 852.0, 675.46875, 0.9365234375]]</t>
+          <t>[[0.0, 0.0, 489.125, 295.25, 158.375, 271.5, 0.9411430358886719, 1107.0, 352.96875, 0.97021484375, 1110.0, 344.296875, 0.47802734375, 1099.0, 341.25, 0.97705078125, 1091.0, 348.515625, 0.028106689453125, 1063.0, 340.3125, 0.947265625, 1062.0, 404.53125, 0.97802734375, 1031.0, 382.265625, 0.98486328125, 1037.0, 496.40625, 0.93115234375, 964.0, 438.984375, 0.9716796875, 1086.0, 546.5625, 0.927734375, 994.0, 521.25, 0.96435546875, 1009.5, 546.09375, 0.98583984375, 974.5, 535.3125, 0.98779296875, 1002.0, 669.375, 0.9755859375, 979.0, 664.21875, 0.97900390625, 932.0, 779.0625, 0.9306640625, 852.0, 675.46875, 0.9365234375]]</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 511.140625, 291.375, 151.5, 280.5, 0.9429981708526611, 1129.0, 338.203125, 0.98876953125, 1132.0, 329.53125, 0.56640625, 1120.0, 326.71875, 0.99267578125, 1119.0, 333.28125, 0.017913818359375, 1084.0, 324.84375, 0.78857421875, 1088.0, 392.34375, 0.9599609375, 1049.0, 367.5, 0.96630859375, 1068.0, 479.53125, 0.90869140625, 974.5, 418.125, 0.9375, 1122.0, 522.65625, 0.8759765625, 1006.0, 500.625, 0.9111328125, 1038.0, 537.1875, 0.97412109375, 1009.0, 524.53125, 0.97607421875, 1017.5, 660.9375, 0.939453125, 1015.0, 650.15625, 0.9423828125, 944.0, 766.875, 0.86083984375, 901.0, 695.15625, 0.86376953125]]</t>
+          <t>[[0.0, 0.0, 511.140625, 291.375, 151.5, 280.5, 0.9429981708526611, 1129.0, 338.203125, 0.98876953125, 1132.0, 329.53125, 0.56591796875, 1120.0, 326.71875, 0.99267578125, 1119.0, 333.28125, 0.017913818359375, 1084.0, 324.84375, 0.78857421875, 1088.0, 392.34375, 0.9599609375, 1049.0, 367.265625, 0.96630859375, 1068.0, 479.53125, 0.90869140625, 974.5, 418.125, 0.9375, 1122.0, 522.65625, 0.8759765625, 1006.0, 500.625, 0.9111328125, 1038.0, 537.1875, 0.97412109375, 1009.0, 524.53125, 0.97607421875, 1017.5, 660.9375, 0.939453125, 1015.5, 650.15625, 0.9423828125, 944.0, 766.875, 0.86083984375, 901.0, 695.15625, 0.86376953125]]</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 531.59375, 286.375, 140.5, 285.75, 0.9406628608703613, 1152.0, 327.1875, 0.98291015625, 1156.0, 318.75, 0.5771484375, 1145.0, 314.53125, 0.9873046875, 1135.0, 322.734375, 0.029754638671875, 1110.0, 310.546875, 0.9462890625, 1112.0, 381.5625, 0.97802734375, 1074.0, 355.3125, 0.98388671875, 1091.0, 468.046875, 0.921875, 992.0, 397.265625, 0.96728515625, 1151.0, 497.34375, 0.91259765625, 1023.5, 477.421875, 0.958984375, 1055.0, 525.46875, 0.98193359375, 1037.0, 519.375, 0.984375, 1020.5, 645.9375, 0.95947265625, 1052.0, 647.8125, 0.96630859375, 964.0, 751.40625, 0.869140625, 959.5, 743.4375, 0.87939453125]]</t>
+          <t>[[0.0, 0.0, 531.59375, 286.375, 140.5, 285.75, 0.9406628608703613, 1152.0, 327.1875, 0.98291015625, 1156.0, 318.75, 0.5771484375, 1145.0, 314.53125, 0.9873046875, 1135.0, 322.734375, 0.029754638671875, 1110.0, 310.546875, 0.9462890625, 1112.0, 381.5625, 0.97802734375, 1074.0, 355.3125, 0.98388671875, 1091.0, 468.046875, 0.921875, 992.0, 397.5, 0.96728515625, 1151.0, 497.34375, 0.91259765625, 1023.5, 477.421875, 0.958984375, 1055.0, 525.46875, 0.98193359375, 1037.0, 519.375, 0.984375, 1021.0, 645.9375, 0.95947265625, 1052.0, 647.8125, 0.96630859375, 964.0, 750.9375, 0.869140625, 959.5, 743.4375, 0.87939453125]]</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 540.125, 287.4375, 149.25, 296.0, 0.9396286010742188, 1177.0, 315.9375, 0.9892578125, 1181.0, 306.796875, 0.630859375, 1167.0, 303.984375, 0.9921875, 1169.0, 312.421875, 0.0224151611328125, 1132.0, 304.21875, 0.78857421875, 1139.0, 373.359375, 0.962890625, 1093.0, 347.8125, 0.96875, 1115.0, 461.015625, 0.91748046875, 1004.5, 384.609375, 0.9423828125, 1177.0, 480.9375, 0.88720703125, 1037.0, 460.3125, 0.916015625, 1081.0, 522.1875, 0.97802734375, 1065.0, 516.5625, 0.9794921875, 1043.0, 645.46875, 0.94873046875, 1094.0, 643.125, 0.953125, 965.0, 743.4375, 0.8740234375, 1038.0, 764.0625, 0.87890625]]</t>
+          <t>[[0.0, 0.0, 540.125, 287.46875, 149.25, 296.0, 0.9396286010742188, 1177.0, 315.9375, 0.9892578125, 1181.0, 306.796875, 0.630859375, 1167.0, 303.984375, 0.9921875, 1169.0, 312.421875, 0.0224151611328125, 1132.0, 304.21875, 0.7890625, 1139.0, 373.359375, 0.962890625, 1093.0, 347.8125, 0.96875, 1115.0, 461.015625, 0.91748046875, 1004.5, 384.609375, 0.9423828125, 1177.0, 480.9375, 0.88720703125, 1037.0, 460.3125, 0.916015625, 1081.0, 522.1875, 0.97802734375, 1065.0, 516.5625, 0.9794921875, 1043.0, 645.46875, 0.94873046875, 1094.0, 643.125, 0.953125, 965.0, 743.4375, 0.8740234375, 1038.0, 764.0625, 0.87890625]]</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 548.75, 287.40625, 154.75, 306.5, 0.9434795379638672, 1201.0, 311.71875, 0.98681640625, 1205.0, 301.875, 0.51318359375, 1192.0, 299.53125, 0.99072265625, 1191.0, 305.15625, 0.0165863037109375, 1157.0, 298.59375, 0.783203125, 1165.0, 365.15625, 0.96044921875, 1116.0, 345.234375, 0.96923828125, 1141.0, 453.28125, 0.91357421875, 1029.0, 377.578125, 0.9453125, 1201.0, 463.59375, 0.8828125, 1066.0, 452.34375, 0.91845703125, 1116.0, 518.4375, 0.9794921875, 1098.0, 515.625, 0.98193359375, 1065.0, 639.84375, 0.95458984375, 1129.0, 647.8125, 0.96044921875, 979.0, 731.25, 0.88916015625, 1117.0, 784.6875, 0.89599609375]]</t>
+          <t>[[0.0, 0.0, 548.8125, 287.40625, 154.5, 306.5, 0.9434795379638672, 1201.0, 311.71875, 0.98681640625, 1205.0, 301.875, 0.5126953125, 1192.0, 299.53125, 0.99072265625, 1191.0, 305.15625, 0.0165252685546875, 1157.0, 298.59375, 0.78369140625, 1165.0, 365.15625, 0.96044921875, 1116.0, 345.46875, 0.96923828125, 1141.0, 453.28125, 0.91357421875, 1029.0, 377.578125, 0.9453125, 1201.0, 463.59375, 0.8828125, 1066.0, 452.34375, 0.9189453125, 1116.0, 518.4375, 0.9794921875, 1098.0, 515.625, 0.98193359375, 1065.0, 639.84375, 0.95458984375, 1129.0, 647.8125, 0.96044921875, 979.0, 731.25, 0.88916015625, 1117.0, 784.6875, 0.896484375]]</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 558.125, 288.0, 156.75, 310.0, 0.9458863735198975, 1226.0, 311.015625, 0.9873046875, 1231.0, 300.703125, 0.51611328125, 1217.0, 299.0625, 0.99072265625, 1217.0, 303.984375, 0.015777587890625, 1180.0, 297.1875, 0.78515625, 1188.0, 366.5625, 0.95556640625, 1143.0, 345.9375, 0.9697265625, 1163.0, 452.578125, 0.90185546875, 1052.0, 378.28125, 0.94580078125, 1228.0, 457.03125, 0.87109375, 1090.0, 452.578125, 0.91845703125, 1148.0, 520.3125, 0.97802734375, 1132.0, 516.5625, 0.98193359375, 1096.0, 641.71875, 0.95556640625, 1165.0, 652.5, 0.96337890625, 997.0, 727.03125, 0.8955078125, 1190.0, 794.0625, 0.9052734375]]</t>
+          <t>[[0.0, 0.0, 558.125, 288.0, 156.75, 310.0, 0.9458863735198975, 1226.0, 311.015625, 0.9873046875, 1231.0, 300.703125, 0.5166015625, 1217.0, 299.0625, 0.99072265625, 1217.0, 303.984375, 0.015777587890625, 1180.0, 297.1875, 0.78515625, 1188.0, 366.5625, 0.95556640625, 1143.0, 345.9375, 0.9697265625, 1164.0, 452.578125, 0.90185546875, 1052.0, 378.28125, 0.94580078125, 1228.0, 457.03125, 0.87109375, 1090.0, 452.578125, 0.91845703125, 1148.0, 520.3125, 0.97802734375, 1132.0, 516.5625, 0.98193359375, 1096.0, 642.1875, 0.95556640625, 1165.0, 652.5, 0.96337890625, 997.0, 727.03125, 0.89501953125, 1190.0, 794.0625, 0.9052734375]]</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 575.1875, 291.5625, 171.875, 313.75, 0.950218677520752, 1255.0, 311.953125, 0.9892578125, 1258.0, 302.34375, 0.50927734375, 1245.0, 300.234375, 0.99267578125, 1240.0, 306.09375, 0.0154266357421875, 1207.0, 300.9375, 0.79248046875, 1216.0, 369.375, 0.96240234375, 1169.0, 350.859375, 0.96923828125, 1192.0, 458.203125, 0.9140625, 1079.0, 390.0, 0.94189453125, 1252.0, 461.25, 0.88330078125, 1116.0, 462.65625, 0.91650390625, 1175.0, 525.9375, 0.97802734375, 1162.0, 524.0625, 0.97998046875, 1120.0, 647.34375, 0.9560546875, 1210.0, 656.25, 0.96044921875, 1012.0, 724.6875, 0.89306640625, 1250.0, 798.75, 0.89892578125]]</t>
+          <t>[[0.0, 0.0, 575.1875, 291.5625, 171.875, 313.75, 0.950218677520752, 1255.0, 311.953125, 0.9892578125, 1258.0, 302.34375, 0.50927734375, 1245.0, 300.234375, 0.99267578125, 1240.0, 306.09375, 0.0154266357421875, 1207.0, 300.9375, 0.79248046875, 1216.0, 369.375, 0.96240234375, 1169.0, 350.859375, 0.96923828125, 1192.0, 458.203125, 0.9140625, 1079.0, 390.0, 0.94189453125, 1252.0, 461.25, 0.88330078125, 1116.0, 462.65625, 0.91650390625, 1175.0, 525.9375, 0.97802734375, 1162.0, 524.0625, 0.97998046875, 1120.0, 647.34375, 0.9560546875, 1210.0, 656.25, 0.96044921875, 1012.0, 724.6875, 0.89306640625, 1250.0, 798.75, 0.8984375]]</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 593.625, 295.46875, 186.0, 317.75, 0.9445042610168457, 1282.0, 322.03125, 0.9853515625, 1285.0, 311.25, 0.52294921875, 1274.0, 309.84375, 0.986328125, 1260.0, 313.125, 0.0252685546875, 1235.0, 307.734375, 0.94921875, 1247.0, 371.71875, 0.9765625, 1196.0, 361.40625, 0.98486328125, 1221.0, 459.375, 0.92529296875, 1113.0, 410.859375, 0.97412109375, 1282.0, 474.609375, 0.9189453125, 1154.0, 480.46875, 0.96630859375, 1213.0, 533.90625, 0.98583984375, 1195.0, 533.90625, 0.98876953125, 1158.0, 657.1875, 0.9765625, 1253.0, 669.84375, 0.9833984375, 1036.0, 722.34375, 0.93408203125, 1292.0, 811.40625, 0.94482421875]]</t>
+          <t>[[0.0, 0.0, 593.625, 295.46875, 186.0, 317.75, 0.9445042610168457, 1282.0, 322.03125, 0.9853515625, 1285.0, 311.25, 0.52294921875, 1274.0, 309.609375, 0.986328125, 1260.0, 313.125, 0.0252685546875, 1235.0, 307.734375, 0.94921875, 1247.0, 371.71875, 0.9765625, 1196.0, 361.40625, 0.98486328125, 1221.0, 459.375, 0.92529296875, 1113.0, 410.859375, 0.9736328125, 1282.0, 474.609375, 0.9189453125, 1154.0, 480.46875, 0.96630859375, 1213.0, 533.90625, 0.98583984375, 1195.0, 533.90625, 0.98876953125, 1158.0, 657.1875, 0.9765625, 1253.0, 669.84375, 0.9833984375, 1036.0, 722.34375, 0.93408203125, 1292.0, 811.40625, 0.94482421875]]</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 601.375, 300.09375, 172.0, 320.0, 0.9445042610168457, 1309.0, 329.0625, 0.97705078125, 1313.0, 318.75, 0.484130859375, 1301.0, 316.875, 0.9814453125, 1288.0, 322.03125, 0.029205322265625, 1261.0, 316.171875, 0.95263671875, 1268.0, 384.140625, 0.9755859375, 1226.0, 374.53125, 0.98583984375, 1250.0, 467.8125, 0.91943359375, 1147.0, 437.109375, 0.97412109375, 1304.0, 497.8125, 0.9140625, 1190.0, 511.40625, 0.96533203125, 1240.0, 547.96875, 0.98486328125, 1230.0, 548.90625, 0.98828125, 1195.0, 672.1875, 0.9736328125, 1297.0, 680.625, 0.98193359375, 1068.0, 727.03125, 0.9267578125, 1304.0, 824.53125, 0.939453125]]</t>
+          <t>[[0.0, 0.0, 601.375, 300.078125, 172.0, 320.0, 0.9445042610168457, 1309.0, 329.0625, 0.9765625, 1313.0, 318.75, 0.48388671875, 1301.0, 316.640625, 0.9814453125, 1288.0, 322.03125, 0.0292510986328125, 1261.0, 316.171875, 0.95263671875, 1268.0, 384.140625, 0.9755859375, 1226.0, 374.53125, 0.98583984375, 1250.0, 467.8125, 0.91943359375, 1147.0, 437.109375, 0.97412109375, 1304.0, 497.8125, 0.91357421875, 1190.0, 511.40625, 0.96533203125, 1240.0, 547.96875, 0.98486328125, 1230.0, 548.90625, 0.98828125, 1195.0, 672.1875, 0.9736328125, 1297.0, 680.625, 0.98193359375, 1068.0, 727.03125, 0.9267578125, 1304.0, 824.53125, 0.939453125]]</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 613.015625, 301.296875, 151.75, 319.5, 0.9406628608703613, 1336.0, 333.75, 0.9814453125, 1340.0, 322.5, 0.46630859375, 1328.0, 320.15625, 0.98779296875, 1315.0, 323.671875, 0.0212860107421875, 1289.0, 319.21875, 0.95849609375, 1293.0, 384.375, 0.978515625, 1255.0, 383.90625, 0.98681640625, 1277.0, 478.125, 0.92138671875, 1193.0, 466.640625, 0.97509765625, 1327.0, 519.84375, 0.91455078125, 1237.0, 543.28125, 0.9658203125, 1275.0, 555.0, 0.9853515625, 1263.0, 556.40625, 0.98828125, 1242.0, 685.3125, 0.97412109375, 1328.0, 685.78125, 0.98193359375, 1114.0, 730.3125, 0.927734375, 1308.0, 829.6875, 0.94189453125]]</t>
+          <t>[[0.0, 0.0, 613.046875, 301.296875, 151.75, 319.5, 0.9406628608703613, 1336.0, 333.75, 0.9814453125, 1340.0, 322.265625, 0.465087890625, 1328.0, 320.15625, 0.98779296875, 1315.0, 323.4375, 0.0212860107421875, 1289.0, 319.21875, 0.95849609375, 1293.0, 384.140625, 0.978515625, 1255.0, 383.90625, 0.98681640625, 1277.0, 478.125, 0.92138671875, 1193.0, 466.640625, 0.97509765625, 1327.0, 519.84375, 0.91455078125, 1237.0, 543.28125, 0.9658203125, 1275.0, 555.0, 0.9853515625, 1263.0, 556.40625, 0.98828125, 1242.0, 685.3125, 0.97412109375, 1328.0, 685.3125, 0.98193359375, 1114.0, 730.3125, 0.927734375, 1308.0, 829.6875, 0.94189453125]]</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 628.0625, 301.21875, 136.0, 318.25, 0.9358611106872559, 1363.0, 333.046875, 0.943359375, 1364.0, 321.5625, 0.2354736328125, 1356.0, 320.15625, 0.97021484375, 1336.0, 322.734375, 0.0165252685546875, 1317.0, 318.28125, 0.9560546875, 1316.0, 386.25, 0.97265625, 1282.0, 386.25, 0.98583984375, 1306.0, 481.875, 0.8857421875, 1237.0, 477.890625, 0.9736328125, 1348.0, 526.875, 0.87353515625, 1298.0, 548.90625, 0.96044921875, 1303.0, 560.625, 0.98095703125, 1288.0, 563.4375, 0.986328125, 1292.0, 690.9375, 0.9638671875, 1348.0, 690.9375, 0.97802734375, 1161.0, 737.8125, 0.908203125, 1308.0, 825.9375, 0.9306640625]]</t>
+          <t>[[0.0, 0.0, 628.0625, 301.21875, 136.0, 318.25, 0.9358611106872559, 1363.0, 333.046875, 0.943359375, 1364.0, 321.5625, 0.2354736328125, 1356.0, 320.15625, 0.97021484375, 1336.0, 322.734375, 0.0165252685546875, 1317.0, 318.28125, 0.9560546875, 1316.0, 386.25, 0.97216796875, 1282.0, 386.25, 0.98583984375, 1306.0, 481.875, 0.8857421875, 1237.0, 477.890625, 0.9736328125, 1348.0, 526.875, 0.87353515625, 1298.0, 548.90625, 0.96044921875, 1303.0, 560.625, 0.98095703125, 1288.0, 563.4375, 0.986328125, 1292.0, 690.9375, 0.9638671875, 1348.0, 690.9375, 0.9775390625, 1161.0, 737.8125, 0.908203125, 1308.0, 825.9375, 0.9306640625]]</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 647.65625, 299.34375, 123.8125, 321.75, 0.9425835609436035, 1388.0, 330.0, 0.96923828125, 1391.0, 318.046875, 0.351806640625, 1380.0, 315.9375, 0.984375, 1368.0, 319.21875, 0.01512908935546875, 1343.0, 313.125, 0.96044921875, 1336.0, 377.8125, 0.9140625, 1306.0, 379.453125, 0.9833984375, 1323.0, 473.671875, 0.47119140625, 1276.0, 476.71875, 0.970703125, 1372.0, 525.0, 0.463134765625, 1359.0, 526.875, 0.94482421875, 1329.0, 549.84375, 0.9541015625, 1307.0, 553.125, 0.9814453125, 1345.0, 690.0, 0.935546875, 1360.0, 694.6875, 0.978515625, 1216.0, 748.125, 0.890625, 1309.0, 823.125, 0.94677734375]]</t>
+          <t>[[0.0, 0.0, 647.65625, 299.328125, 123.8125, 321.75, 0.9425835609436035, 1388.0, 329.53125, 0.96923828125, 1391.0, 318.046875, 0.351806640625, 1380.0, 315.9375, 0.984375, 1368.0, 319.21875, 0.01519012451171875, 1343.0, 313.125, 0.96044921875, 1336.0, 377.8125, 0.9140625, 1306.0, 379.453125, 0.9833984375, 1323.0, 473.671875, 0.4716796875, 1276.0, 476.71875, 0.970703125, 1372.0, 525.0, 0.46337890625, 1359.0, 526.875, 0.94482421875, 1329.0, 549.84375, 0.9541015625, 1307.0, 553.125, 0.9814453125, 1345.0, 690.0, 0.935546875, 1360.0, 694.21875, 0.978515625, 1216.0, 748.125, 0.890625, 1309.0, 823.125, 0.94677734375]]</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>[[0.0, 0.0, 675.296875, 297.4375, 118.4375, 331.0, 0.9358611106872559, 1414.0, 322.734375, 0.943359375, 1417.0, 311.25, 0.240966796875, 1407.0, 309.375, 0.970703125, 1390.0, 311.25, 0.01763916015625, 1371.0, 304.6875, 0.95703125, 1361.0, 370.3125, 0.91796875, 1334.0, 369.84375, 0.9814453125, 1346.0, 468.984375, 0.491455078125, 1317.0, 465.46875, 0.96826171875, 1401.0, 518.4375, 0.477294921875, 1413.0, 498.28125, 0.94384765625, 1364.0, 543.75, 0.95849609375, 1335.0, 545.625, 0.98193359375, 1398.0, 681.09375, 0.94873046875, 1371.0, 688.59375, 0.98193359375, 1284.0, 766.875, 0.91748046875, 1312.0, 823.125, 0.9580078125]]</t>
+          <t>[[0.0, 0.0, 675.296875, 297.4375, 118.3125, 331.0, 0.9358611106872559, 1414.0, 322.734375, 0.943359375, 1417.0, 311.015625, 0.2406005859375, 1407.0, 309.375, 0.970703125, 1390.0, 311.25, 0.017578125, 1371.0, 304.6875, 0.95751953125, 1361.0, 370.3125, 0.91796875, 1334.0, 369.84375, 0.9814453125, 1346.0, 468.75, 0.491455078125, 1317.0, 465.46875, 0.96826171875, 1401.0, 518.4375, 0.477294921875, 1413.0, 498.28125, 0.94384765625, 1364.0, 543.75, 0.95849609375, 1335.0, 545.625, 0.98193359375, 1398.0, 681.09375, 0.94873046875, 1371.0, 688.59375, 0.98193359375, 1284.0, 766.875, 0.91748046875, 1312.0, 823.125, 0.9580078125]]</t>
         </is>
       </c>
     </row>

</xml_diff>